<commit_message>
interactive app and control flow
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="6" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="references-latest" sheetId="28" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5492" uniqueCount="3009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5495" uniqueCount="3012">
   <si>
     <t>USER</t>
   </si>
@@ -9431,6 +9431,15 @@
   </si>
   <si>
     <t>false ex-or false</t>
+  </si>
+  <si>
+    <t>decision making</t>
+  </si>
+  <si>
+    <t>WELCOME !!!</t>
+  </si>
+  <si>
+    <t>if-else-if</t>
   </si>
 </sst>
 </file>
@@ -10125,7 +10134,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="407">
+  <cellXfs count="408">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -10847,6 +10856,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10883,18 +10898,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10908,6 +10911,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10950,9 +10965,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -17501,8 +17513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O187"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17574,7 +17586,9 @@
     <row r="4" spans="1:15">
       <c r="A4" s="54"/>
       <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
+      <c r="C4" s="370" t="s">
+        <v>3009</v>
+      </c>
       <c r="D4" s="54"/>
       <c r="E4" s="124" t="s">
         <v>2343</v>
@@ -17647,7 +17661,9 @@
         <v>391</v>
       </c>
       <c r="G7" s="54"/>
-      <c r="H7" s="62"/>
+      <c r="H7" s="62" t="s">
+        <v>3010</v>
+      </c>
       <c r="J7" s="159" t="s">
         <v>1512</v>
       </c>
@@ -17753,7 +17769,9 @@
       <c r="C12" s="54"/>
       <c r="D12" s="54"/>
       <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
+      <c r="F12" s="124" t="s">
+        <v>3011</v>
+      </c>
       <c r="G12" s="54"/>
       <c r="H12" s="59" t="s">
         <v>380</v>
@@ -23906,8 +23924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD165"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30:N33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23951,13 +23969,13 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1">
-      <c r="H3" s="376" t="s">
+      <c r="H3" s="378" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="377"/>
-      <c r="J3" s="377"/>
-      <c r="K3" s="377"/>
-      <c r="L3" s="378"/>
+      <c r="I3" s="379"/>
+      <c r="J3" s="379"/>
+      <c r="K3" s="379"/>
+      <c r="L3" s="380"/>
       <c r="P3" t="s">
         <v>2376</v>
       </c>
@@ -24000,20 +24018,20 @@
         <v>2373</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="379" t="s">
+      <c r="G6" s="381" t="s">
         <v>2371</v>
       </c>
-      <c r="H6" s="380"/>
+      <c r="H6" s="382"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="379" t="s">
+      <c r="J6" s="381" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="380"/>
+      <c r="K6" s="382"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="379" t="s">
+      <c r="M6" s="381" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="380"/>
+      <c r="N6" s="382"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1">
       <c r="D7" s="122" t="s">
@@ -24034,20 +24052,20 @@
     </row>
     <row r="8" spans="1:18">
       <c r="F8" s="4"/>
-      <c r="G8" s="381" t="s">
+      <c r="G8" s="383" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="382"/>
+      <c r="H8" s="384"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="381" t="s">
+      <c r="J8" s="383" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="382"/>
+      <c r="K8" s="384"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="381" t="s">
+      <c r="M8" s="383" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="382"/>
+      <c r="N8" s="384"/>
       <c r="Q8" s="139"/>
     </row>
     <row r="9" spans="1:18">
@@ -24072,17 +24090,17 @@
       <c r="B10" t="s">
         <v>298</v>
       </c>
-      <c r="F10" s="372" t="s">
+      <c r="F10" s="374" t="s">
         <v>2789</v>
       </c>
-      <c r="G10" s="373"/>
-      <c r="H10" s="373"/>
-      <c r="I10" s="373"/>
-      <c r="J10" s="373"/>
-      <c r="K10" s="373"/>
-      <c r="L10" s="373"/>
-      <c r="M10" s="373"/>
-      <c r="N10" s="373"/>
+      <c r="G10" s="375"/>
+      <c r="H10" s="375"/>
+      <c r="I10" s="375"/>
+      <c r="J10" s="375"/>
+      <c r="K10" s="375"/>
+      <c r="L10" s="375"/>
+      <c r="M10" s="375"/>
+      <c r="N10" s="375"/>
       <c r="P10" t="s">
         <v>2791</v>
       </c>
@@ -24092,15 +24110,15 @@
       <c r="B11" t="s">
         <v>284</v>
       </c>
-      <c r="F11" s="374"/>
-      <c r="G11" s="375"/>
-      <c r="H11" s="375"/>
-      <c r="I11" s="375"/>
-      <c r="J11" s="375"/>
-      <c r="K11" s="375"/>
-      <c r="L11" s="375"/>
-      <c r="M11" s="375"/>
-      <c r="N11" s="375"/>
+      <c r="F11" s="376"/>
+      <c r="G11" s="377"/>
+      <c r="H11" s="377"/>
+      <c r="I11" s="377"/>
+      <c r="J11" s="377"/>
+      <c r="K11" s="377"/>
+      <c r="L11" s="377"/>
+      <c r="M11" s="377"/>
+      <c r="N11" s="377"/>
       <c r="P11" t="s">
         <v>2792</v>
       </c>
@@ -24354,10 +24372,10 @@
       <c r="C23" t="s">
         <v>2720</v>
       </c>
-      <c r="D23" s="370" t="s">
+      <c r="D23" s="372" t="s">
         <v>1076</v>
       </c>
-      <c r="E23" s="371"/>
+      <c r="E23" s="373"/>
       <c r="F23" s="138"/>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
@@ -25677,7 +25695,7 @@
       </c>
       <c r="I21" s="44"/>
       <c r="J21" s="45"/>
-      <c r="K21" s="397" t="s">
+      <c r="K21" s="399" t="s">
         <v>2475</v>
       </c>
       <c r="L21" s="48"/>
@@ -25704,7 +25722,7 @@
       <c r="J22" s="48" t="s">
         <v>894</v>
       </c>
-      <c r="K22" s="398"/>
+      <c r="K22" s="400"/>
       <c r="L22" s="48"/>
       <c r="M22" s="49"/>
     </row>
@@ -25729,7 +25747,7 @@
       <c r="J23" s="51">
         <v>333</v>
       </c>
-      <c r="K23" s="398"/>
+      <c r="K23" s="400"/>
       <c r="L23" s="48"/>
       <c r="M23" s="49"/>
     </row>
@@ -25750,7 +25768,7 @@
       <c r="H24" s="48"/>
       <c r="I24" s="48"/>
       <c r="J24" s="48"/>
-      <c r="K24" s="398"/>
+      <c r="K24" s="400"/>
       <c r="L24" s="48"/>
       <c r="M24" s="49"/>
     </row>
@@ -25767,7 +25785,7 @@
       </c>
       <c r="I25" s="44"/>
       <c r="J25" s="45"/>
-      <c r="K25" s="398"/>
+      <c r="K25" s="400"/>
       <c r="L25" s="48"/>
       <c r="M25" s="49"/>
     </row>
@@ -25782,7 +25800,7 @@
       <c r="J26" s="48" t="s">
         <v>2462</v>
       </c>
-      <c r="K26" s="398"/>
+      <c r="K26" s="400"/>
       <c r="L26" s="48"/>
       <c r="M26" s="49"/>
     </row>
@@ -25797,7 +25815,7 @@
       <c r="J27" s="51">
         <v>234</v>
       </c>
-      <c r="K27" s="398"/>
+      <c r="K27" s="400"/>
       <c r="L27" s="48"/>
       <c r="M27" s="49"/>
     </row>
@@ -25811,7 +25829,7 @@
       <c r="H28" s="48"/>
       <c r="I28" s="48"/>
       <c r="J28" s="48"/>
-      <c r="K28" s="398"/>
+      <c r="K28" s="400"/>
       <c r="L28" s="48"/>
       <c r="M28" s="49"/>
     </row>
@@ -25827,7 +25845,7 @@
       </c>
       <c r="I29" s="44"/>
       <c r="J29" s="45"/>
-      <c r="K29" s="398"/>
+      <c r="K29" s="400"/>
       <c r="L29" s="48"/>
       <c r="M29" s="49"/>
     </row>
@@ -25845,7 +25863,7 @@
       <c r="J30" s="48" t="s">
         <v>2463</v>
       </c>
-      <c r="K30" s="398"/>
+      <c r="K30" s="400"/>
       <c r="L30" s="48"/>
       <c r="M30" s="49"/>
     </row>
@@ -25860,7 +25878,7 @@
       <c r="J31" s="51">
         <v>345</v>
       </c>
-      <c r="K31" s="399"/>
+      <c r="K31" s="401"/>
       <c r="L31" s="48"/>
       <c r="M31" s="49"/>
     </row>
@@ -42529,10 +42547,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="2:13">
-      <c r="B1" s="400" t="s">
+      <c r="B1" s="402" t="s">
         <v>2682</v>
       </c>
-      <c r="C1" s="400"/>
+      <c r="C1" s="402"/>
       <c r="E1" t="s">
         <v>2683</v>
       </c>
@@ -44896,11 +44914,11 @@
       <c r="B223" t="s">
         <v>1516</v>
       </c>
-      <c r="D223" s="383" t="s">
+      <c r="D223" s="390" t="s">
         <v>42</v>
       </c>
-      <c r="E223" s="385"/>
-      <c r="F223" s="384"/>
+      <c r="E223" s="392"/>
+      <c r="F223" s="391"/>
       <c r="H223" s="31"/>
       <c r="I223" s="32"/>
       <c r="K223" s="31"/>
@@ -44952,19 +44970,19 @@
       <c r="B227" t="s">
         <v>1936</v>
       </c>
-      <c r="D227" s="383" t="s">
+      <c r="D227" s="390" t="s">
         <v>1538</v>
       </c>
-      <c r="E227" s="385"/>
-      <c r="F227" s="384"/>
-      <c r="H227" s="383" t="s">
+      <c r="E227" s="392"/>
+      <c r="F227" s="391"/>
+      <c r="H227" s="390" t="s">
         <v>1541</v>
       </c>
-      <c r="I227" s="384"/>
-      <c r="K227" s="383" t="s">
+      <c r="I227" s="391"/>
+      <c r="K227" s="390" t="s">
         <v>1540</v>
       </c>
-      <c r="L227" s="384"/>
+      <c r="L227" s="391"/>
     </row>
     <row r="228" spans="2:12">
       <c r="D228" s="31" t="s">
@@ -45211,7 +45229,7 @@
       </c>
     </row>
     <row r="273" spans="2:15">
-      <c r="D273" s="386" t="s">
+      <c r="D273" s="393" t="s">
         <v>2767</v>
       </c>
       <c r="F273" s="162" t="s">
@@ -45219,22 +45237,22 @@
       </c>
     </row>
     <row r="274" spans="2:15">
-      <c r="D274" s="386"/>
+      <c r="D274" s="393"/>
     </row>
     <row r="275" spans="2:15">
-      <c r="D275" s="386"/>
+      <c r="D275" s="393"/>
       <c r="F275" t="s">
         <v>2766</v>
       </c>
     </row>
     <row r="276" spans="2:15">
-      <c r="D276" s="386"/>
+      <c r="D276" s="393"/>
       <c r="K276" t="s">
         <v>2782</v>
       </c>
     </row>
     <row r="277" spans="2:15">
-      <c r="D277" s="386"/>
+      <c r="D277" s="393"/>
       <c r="F277" s="162" t="s">
         <v>1936</v>
       </c>
@@ -45249,7 +45267,7 @@
       </c>
     </row>
     <row r="278" spans="2:15">
-      <c r="D278" s="386"/>
+      <c r="D278" s="393"/>
       <c r="I278" t="s">
         <v>2784</v>
       </c>
@@ -45335,14 +45353,14 @@
       <c r="O286" s="32"/>
     </row>
     <row r="287" spans="2:15">
-      <c r="B287" s="388" t="s">
+      <c r="B287" s="386" t="s">
         <v>2777</v>
       </c>
-      <c r="C287" s="387" t="s">
+      <c r="C287" s="385" t="s">
         <v>1532</v>
       </c>
-      <c r="D287" s="387"/>
-      <c r="E287" s="371"/>
+      <c r="D287" s="385"/>
+      <c r="E287" s="373"/>
       <c r="G287" s="31"/>
       <c r="H287" s="25"/>
       <c r="I287" s="25"/>
@@ -45353,7 +45371,7 @@
       <c r="O287" s="32"/>
     </row>
     <row r="288" spans="2:15">
-      <c r="B288" s="372"/>
+      <c r="B288" s="374"/>
       <c r="C288" s="25"/>
       <c r="D288" s="25" t="s">
         <v>1376</v>
@@ -45364,7 +45382,7 @@
       </c>
       <c r="H288" s="25"/>
       <c r="I288" s="25"/>
-      <c r="J288" s="390" t="s">
+      <c r="J288" s="388" t="s">
         <v>2779</v>
       </c>
       <c r="L288" s="31"/>
@@ -45373,7 +45391,7 @@
       <c r="O288" s="32"/>
     </row>
     <row r="289" spans="2:15">
-      <c r="B289" s="372"/>
+      <c r="B289" s="374"/>
       <c r="C289" s="25" t="s">
         <v>2772</v>
       </c>
@@ -45385,49 +45403,49 @@
       <c r="G289" s="31"/>
       <c r="H289" s="25"/>
       <c r="I289" s="25"/>
-      <c r="J289" s="391"/>
+      <c r="J289" s="389"/>
       <c r="L289" s="31" t="s">
         <v>2772</v>
       </c>
       <c r="M289" s="25"/>
       <c r="N289" s="25"/>
-      <c r="O289" s="390" t="s">
+      <c r="O289" s="388" t="s">
         <v>2778</v>
       </c>
     </row>
     <row r="290" spans="2:15">
-      <c r="B290" s="372"/>
+      <c r="B290" s="374"/>
       <c r="C290" s="25"/>
       <c r="D290" s="25"/>
       <c r="E290" s="32"/>
-      <c r="G290" s="389" t="s">
+      <c r="G290" s="387" t="s">
         <v>2780</v>
       </c>
-      <c r="H290" s="387"/>
-      <c r="I290" s="387"/>
-      <c r="J290" s="391"/>
+      <c r="H290" s="385"/>
+      <c r="I290" s="385"/>
+      <c r="J290" s="389"/>
       <c r="L290" s="31"/>
       <c r="M290" s="25"/>
       <c r="N290" s="25"/>
-      <c r="O290" s="391"/>
+      <c r="O290" s="389"/>
     </row>
     <row r="291" spans="2:15">
-      <c r="B291" s="372"/>
-      <c r="C291" s="387" t="s">
+      <c r="B291" s="374"/>
+      <c r="C291" s="385" t="s">
         <v>2774</v>
       </c>
-      <c r="D291" s="387"/>
-      <c r="E291" s="371"/>
+      <c r="D291" s="385"/>
+      <c r="E291" s="373"/>
       <c r="G291" s="31"/>
       <c r="H291" s="25"/>
       <c r="I291" s="25"/>
-      <c r="J291" s="391"/>
-      <c r="L291" s="389" t="s">
+      <c r="J291" s="389"/>
+      <c r="L291" s="387" t="s">
         <v>2775</v>
       </c>
-      <c r="M291" s="387"/>
-      <c r="N291" s="387"/>
-      <c r="O291" s="391"/>
+      <c r="M291" s="385"/>
+      <c r="N291" s="385"/>
+      <c r="O291" s="389"/>
     </row>
     <row r="292" spans="2:15">
       <c r="B292" s="31"/>
@@ -45441,7 +45459,7 @@
       <c r="L292" s="31"/>
       <c r="M292" s="25"/>
       <c r="N292" s="25"/>
-      <c r="O292" s="391"/>
+      <c r="O292" s="389"/>
     </row>
     <row r="293" spans="2:15">
       <c r="B293" s="31"/>
@@ -45538,6 +45556,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="H227:I227"/>
+    <mergeCell ref="K227:L227"/>
+    <mergeCell ref="D227:F227"/>
+    <mergeCell ref="D223:F223"/>
+    <mergeCell ref="D273:D278"/>
     <mergeCell ref="C287:E287"/>
     <mergeCell ref="C291:E291"/>
     <mergeCell ref="B287:B291"/>
@@ -45545,11 +45568,6 @@
     <mergeCell ref="O289:O292"/>
     <mergeCell ref="J288:J291"/>
     <mergeCell ref="G290:I290"/>
-    <mergeCell ref="H227:I227"/>
-    <mergeCell ref="K227:L227"/>
-    <mergeCell ref="D227:F227"/>
-    <mergeCell ref="D223:F223"/>
-    <mergeCell ref="D273:D278"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -45781,18 +45799,18 @@
   <sheetData>
     <row r="2" spans="2:17" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:17" ht="15.75" thickBot="1">
-      <c r="B3" s="401" t="s">
+      <c r="B3" s="403" t="s">
         <v>2707</v>
       </c>
-      <c r="C3" s="402"/>
-      <c r="D3" s="402"/>
-      <c r="E3" s="402"/>
-      <c r="F3" s="402"/>
-      <c r="G3" s="402"/>
-      <c r="H3" s="402"/>
-      <c r="I3" s="402"/>
-      <c r="J3" s="402"/>
-      <c r="K3" s="403"/>
+      <c r="C3" s="404"/>
+      <c r="D3" s="404"/>
+      <c r="E3" s="404"/>
+      <c r="F3" s="404"/>
+      <c r="G3" s="404"/>
+      <c r="H3" s="404"/>
+      <c r="I3" s="404"/>
+      <c r="J3" s="404"/>
+      <c r="K3" s="405"/>
     </row>
     <row r="4" spans="2:17" ht="15.75" thickBot="1">
       <c r="G4" t="s">
@@ -45907,24 +45925,24 @@
       <c r="L12" s="25"/>
     </row>
     <row r="15" spans="2:17">
-      <c r="B15" s="404" t="s">
+      <c r="B15" s="406" t="s">
         <v>2708</v>
       </c>
-      <c r="C15" s="405"/>
-      <c r="D15" s="405"/>
-      <c r="E15" s="405"/>
-      <c r="F15" s="405"/>
-      <c r="G15" s="405"/>
-      <c r="H15" s="405"/>
-      <c r="I15" s="405"/>
-      <c r="J15" s="405"/>
-      <c r="K15" s="405"/>
-      <c r="L15" s="405"/>
-      <c r="M15" s="405"/>
-      <c r="N15" s="405"/>
-      <c r="O15" s="405"/>
-      <c r="P15" s="405"/>
-      <c r="Q15" s="405"/>
+      <c r="C15" s="407"/>
+      <c r="D15" s="407"/>
+      <c r="E15" s="407"/>
+      <c r="F15" s="407"/>
+      <c r="G15" s="407"/>
+      <c r="H15" s="407"/>
+      <c r="I15" s="407"/>
+      <c r="J15" s="407"/>
+      <c r="K15" s="407"/>
+      <c r="L15" s="407"/>
+      <c r="M15" s="407"/>
+      <c r="N15" s="407"/>
+      <c r="O15" s="407"/>
+      <c r="P15" s="407"/>
+      <c r="Q15" s="407"/>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1"/>
     <row r="17" spans="1:17">
@@ -46205,7 +46223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -46630,28 +46648,28 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="B24" s="406">
+      <c r="B24" s="371">
         <v>0</v>
       </c>
-      <c r="C24" s="406">
+      <c r="C24" s="371">
         <v>0</v>
       </c>
-      <c r="D24" s="406">
+      <c r="D24" s="371">
         <v>0</v>
       </c>
-      <c r="E24" s="406">
+      <c r="E24" s="371">
         <v>0</v>
       </c>
-      <c r="F24" s="406">
+      <c r="F24" s="371">
         <v>0</v>
       </c>
-      <c r="G24" s="406">
+      <c r="G24" s="371">
         <v>1</v>
       </c>
-      <c r="H24" s="406">
+      <c r="H24" s="371">
         <v>0</v>
       </c>
-      <c r="I24" s="406">
+      <c r="I24" s="371">
         <v>1</v>
       </c>
       <c r="J24" s="25">
@@ -46841,28 +46859,28 @@
       </c>
     </row>
     <row r="34" spans="2:15">
-      <c r="B34" s="406">
+      <c r="B34" s="371">
         <v>0</v>
       </c>
-      <c r="C34" s="406">
+      <c r="C34" s="371">
         <v>0</v>
       </c>
-      <c r="D34" s="406">
+      <c r="D34" s="371">
         <v>0</v>
       </c>
-      <c r="E34" s="406">
+      <c r="E34" s="371">
         <v>0</v>
       </c>
-      <c r="F34" s="406">
+      <c r="F34" s="371">
         <v>1</v>
       </c>
-      <c r="G34" s="406">
+      <c r="G34" s="371">
         <v>0</v>
       </c>
-      <c r="H34" s="406">
+      <c r="H34" s="371">
         <v>0</v>
       </c>
-      <c r="I34" s="406">
+      <c r="I34" s="371">
         <v>0</v>
       </c>
       <c r="J34" s="25">
@@ -47368,7 +47386,7 @@
       <c r="A10" s="36" t="s">
         <v>2823</v>
       </c>
-      <c r="G10" s="392" t="s">
+      <c r="G10" s="394" t="s">
         <v>2852</v>
       </c>
       <c r="H10" s="36" t="s">
@@ -47381,7 +47399,7 @@
       <c r="K10" s="36" t="s">
         <v>2859</v>
       </c>
-      <c r="L10" s="392" t="s">
+      <c r="L10" s="394" t="s">
         <v>2852</v>
       </c>
       <c r="M10" s="36" t="s">
@@ -47393,7 +47411,7 @@
       <c r="O10" s="72"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="G11" s="392"/>
+      <c r="G11" s="394"/>
       <c r="H11" s="36" t="s">
         <v>2838</v>
       </c>
@@ -47404,7 +47422,7 @@
       <c r="K11" s="36" t="s">
         <v>2861</v>
       </c>
-      <c r="L11" s="392"/>
+      <c r="L11" s="394"/>
       <c r="M11" s="36" t="s">
         <v>132</v>
       </c>
@@ -47417,7 +47435,7 @@
       <c r="B12" s="36" t="s">
         <v>2824</v>
       </c>
-      <c r="G12" s="392"/>
+      <c r="G12" s="394"/>
       <c r="H12" s="36" t="s">
         <v>2846</v>
       </c>
@@ -47428,7 +47446,7 @@
       <c r="K12" s="36" t="s">
         <v>2862</v>
       </c>
-      <c r="L12" s="392"/>
+      <c r="L12" s="394"/>
       <c r="M12" s="36" t="s">
         <v>134</v>
       </c>
@@ -47441,7 +47459,7 @@
       <c r="C13" s="36" t="s">
         <v>2825</v>
       </c>
-      <c r="G13" s="392"/>
+      <c r="G13" s="394"/>
       <c r="H13" s="36" t="s">
         <v>138</v>
       </c>
@@ -47452,7 +47470,7 @@
       <c r="K13" s="36" t="s">
         <v>2863</v>
       </c>
-      <c r="L13" s="392"/>
+      <c r="L13" s="394"/>
       <c r="M13" s="36" t="s">
         <v>2838</v>
       </c>
@@ -47471,7 +47489,7 @@
       <c r="K14" s="36" t="s">
         <v>2857</v>
       </c>
-      <c r="L14" s="392"/>
+      <c r="L14" s="394"/>
       <c r="M14" s="36" t="s">
         <v>134</v>
       </c>
@@ -47520,7 +47538,7 @@
       <c r="H17" s="79"/>
       <c r="I17" s="79"/>
       <c r="J17" s="80"/>
-      <c r="L17" s="394" t="s">
+      <c r="L17" s="396" t="s">
         <v>2853</v>
       </c>
       <c r="M17" s="36" t="s">
@@ -47531,7 +47549,7 @@
       <c r="D18" s="36" t="s">
         <v>2829</v>
       </c>
-      <c r="G18" s="392" t="s">
+      <c r="G18" s="394" t="s">
         <v>2854</v>
       </c>
       <c r="H18" s="36" t="s">
@@ -47541,7 +47559,7 @@
         <v>53</v>
       </c>
       <c r="J18" s="72"/>
-      <c r="L18" s="394"/>
+      <c r="L18" s="396"/>
       <c r="M18" s="36" t="s">
         <v>2856</v>
       </c>
@@ -47550,7 +47568,7 @@
       <c r="C19" s="36" t="s">
         <v>2830</v>
       </c>
-      <c r="G19" s="392"/>
+      <c r="G19" s="394"/>
       <c r="H19" s="36" t="s">
         <v>138</v>
       </c>
@@ -47563,7 +47581,7 @@
       <c r="D20" s="36" t="s">
         <v>2193</v>
       </c>
-      <c r="G20" s="392"/>
+      <c r="G20" s="394"/>
       <c r="H20" s="36" t="s">
         <v>132</v>
       </c>
@@ -47576,7 +47594,7 @@
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickBot="1">
-      <c r="G21" s="393"/>
+      <c r="G21" s="395"/>
       <c r="H21" s="83" t="s">
         <v>137</v>
       </c>
@@ -48361,23 +48379,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="396" t="s">
+      <c r="A1" s="398" t="s">
         <v>2272</v>
       </c>
-      <c r="B1" s="396"/>
-      <c r="C1" s="396"/>
-      <c r="D1" s="396"/>
-      <c r="E1" s="396"/>
-      <c r="F1" s="396"/>
-      <c r="I1" s="396" t="s">
+      <c r="B1" s="398"/>
+      <c r="C1" s="398"/>
+      <c r="D1" s="398"/>
+      <c r="E1" s="398"/>
+      <c r="F1" s="398"/>
+      <c r="I1" s="398" t="s">
         <v>2282</v>
       </c>
-      <c r="J1" s="396"/>
-      <c r="K1" s="396"/>
-      <c r="L1" s="396"/>
-      <c r="M1" s="396"/>
-      <c r="N1" s="396"/>
-      <c r="O1" s="396"/>
+      <c r="J1" s="398"/>
+      <c r="K1" s="398"/>
+      <c r="L1" s="398"/>
+      <c r="M1" s="398"/>
+      <c r="N1" s="398"/>
+      <c r="O1" s="398"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -48527,28 +48545,28 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A12" s="379" t="s">
+      <c r="A12" s="381" t="s">
         <v>2284</v>
       </c>
-      <c r="B12" s="395"/>
-      <c r="C12" s="395"/>
-      <c r="D12" s="395"/>
-      <c r="E12" s="395"/>
-      <c r="F12" s="395"/>
-      <c r="G12" s="395"/>
-      <c r="H12" s="380"/>
-      <c r="I12" s="379" t="s">
+      <c r="B12" s="397"/>
+      <c r="C12" s="397"/>
+      <c r="D12" s="397"/>
+      <c r="E12" s="397"/>
+      <c r="F12" s="397"/>
+      <c r="G12" s="397"/>
+      <c r="H12" s="382"/>
+      <c r="I12" s="381" t="s">
         <v>2284</v>
       </c>
-      <c r="J12" s="395"/>
-      <c r="K12" s="395"/>
-      <c r="L12" s="395"/>
-      <c r="M12" s="395"/>
-      <c r="N12" s="395"/>
-      <c r="O12" s="395"/>
-      <c r="P12" s="395"/>
-      <c r="Q12" s="395"/>
-      <c r="R12" s="380"/>
+      <c r="J12" s="397"/>
+      <c r="K12" s="397"/>
+      <c r="L12" s="397"/>
+      <c r="M12" s="397"/>
+      <c r="N12" s="397"/>
+      <c r="O12" s="397"/>
+      <c r="P12" s="397"/>
+      <c r="Q12" s="397"/>
+      <c r="R12" s="382"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="28" t="s">
@@ -48776,14 +48794,14 @@
       <c r="R21" s="35"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="396" t="s">
+      <c r="A24" s="398" t="s">
         <v>2272</v>
       </c>
-      <c r="B24" s="396"/>
-      <c r="C24" s="396"/>
-      <c r="D24" s="396"/>
-      <c r="E24" s="396"/>
-      <c r="F24" s="396"/>
+      <c r="B24" s="398"/>
+      <c r="C24" s="398"/>
+      <c r="D24" s="398"/>
+      <c r="E24" s="398"/>
+      <c r="F24" s="398"/>
       <c r="H24" s="250" t="s">
         <v>2282</v>
       </c>
@@ -48793,11 +48811,11 @@
       <c r="L24" s="250"/>
       <c r="M24" s="250"/>
       <c r="N24" s="250"/>
-      <c r="P24" s="396" t="s">
+      <c r="P24" s="398" t="s">
         <v>2320</v>
       </c>
-      <c r="Q24" s="396"/>
-      <c r="R24" s="396"/>
+      <c r="Q24" s="398"/>
+      <c r="R24" s="398"/>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="103" t="s">
@@ -49037,28 +49055,28 @@
       </c>
     </row>
     <row r="35" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A35" s="379" t="s">
+      <c r="A35" s="381" t="s">
         <v>2321</v>
       </c>
-      <c r="B35" s="395"/>
-      <c r="C35" s="395"/>
-      <c r="D35" s="395"/>
-      <c r="E35" s="395"/>
-      <c r="F35" s="395"/>
-      <c r="G35" s="395"/>
-      <c r="H35" s="380"/>
-      <c r="I35" s="379" t="s">
+      <c r="B35" s="397"/>
+      <c r="C35" s="397"/>
+      <c r="D35" s="397"/>
+      <c r="E35" s="397"/>
+      <c r="F35" s="397"/>
+      <c r="G35" s="397"/>
+      <c r="H35" s="382"/>
+      <c r="I35" s="381" t="s">
         <v>872</v>
       </c>
-      <c r="J35" s="395"/>
-      <c r="K35" s="395"/>
-      <c r="L35" s="395"/>
-      <c r="M35" s="395"/>
-      <c r="N35" s="395"/>
-      <c r="O35" s="395"/>
-      <c r="P35" s="395"/>
-      <c r="Q35" s="395"/>
-      <c r="R35" s="380"/>
+      <c r="J35" s="397"/>
+      <c r="K35" s="397"/>
+      <c r="L35" s="397"/>
+      <c r="M35" s="397"/>
+      <c r="N35" s="397"/>
+      <c r="O35" s="397"/>
+      <c r="P35" s="397"/>
+      <c r="Q35" s="397"/>
+      <c r="R35" s="382"/>
     </row>
     <row r="36" spans="1:20" ht="15.75" thickBot="1">
       <c r="A36" s="28" t="s">

</xml_diff>

<commit_message>
access privi and final
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -10423,6 +10423,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10436,18 +10448,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -18929,7 +18929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A7:T274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
@@ -42021,11 +42021,11 @@
       <c r="B223" t="s">
         <v>1415</v>
       </c>
-      <c r="D223" s="376" t="s">
+      <c r="D223" s="371" t="s">
         <v>42</v>
       </c>
-      <c r="E223" s="378"/>
-      <c r="F223" s="377"/>
+      <c r="E223" s="373"/>
+      <c r="F223" s="372"/>
       <c r="H223" s="31"/>
       <c r="I223" s="32"/>
       <c r="K223" s="31"/>
@@ -42077,19 +42077,19 @@
       <c r="B227" t="s">
         <v>1769</v>
       </c>
-      <c r="D227" s="376" t="s">
+      <c r="D227" s="371" t="s">
         <v>1437</v>
       </c>
-      <c r="E227" s="378"/>
-      <c r="F227" s="377"/>
-      <c r="H227" s="376" t="s">
+      <c r="E227" s="373"/>
+      <c r="F227" s="372"/>
+      <c r="H227" s="371" t="s">
         <v>1440</v>
       </c>
-      <c r="I227" s="377"/>
-      <c r="K227" s="376" t="s">
+      <c r="I227" s="372"/>
+      <c r="K227" s="371" t="s">
         <v>1439</v>
       </c>
-      <c r="L227" s="377"/>
+      <c r="L227" s="372"/>
     </row>
     <row r="228" spans="2:12">
       <c r="D228" s="31" t="s">
@@ -42336,7 +42336,7 @@
       </c>
     </row>
     <row r="273" spans="2:15">
-      <c r="D273" s="379" t="s">
+      <c r="D273" s="374" t="s">
         <v>2531</v>
       </c>
       <c r="F273" s="159" t="s">
@@ -42344,22 +42344,22 @@
       </c>
     </row>
     <row r="274" spans="2:15">
-      <c r="D274" s="379"/>
+      <c r="D274" s="374"/>
     </row>
     <row r="275" spans="2:15">
-      <c r="D275" s="379"/>
+      <c r="D275" s="374"/>
       <c r="F275" t="s">
         <v>2530</v>
       </c>
     </row>
     <row r="276" spans="2:15">
-      <c r="D276" s="379"/>
+      <c r="D276" s="374"/>
       <c r="K276" t="s">
         <v>2546</v>
       </c>
     </row>
     <row r="277" spans="2:15">
-      <c r="D277" s="379"/>
+      <c r="D277" s="374"/>
       <c r="F277" s="159" t="s">
         <v>1769</v>
       </c>
@@ -42374,7 +42374,7 @@
       </c>
     </row>
     <row r="278" spans="2:15">
-      <c r="D278" s="379"/>
+      <c r="D278" s="374"/>
       <c r="I278" t="s">
         <v>2548</v>
       </c>
@@ -42460,13 +42460,13 @@
       <c r="O286" s="32"/>
     </row>
     <row r="287" spans="2:15">
-      <c r="B287" s="372" t="s">
+      <c r="B287" s="376" t="s">
         <v>2541</v>
       </c>
-      <c r="C287" s="371" t="s">
+      <c r="C287" s="375" t="s">
         <v>1431</v>
       </c>
-      <c r="D287" s="371"/>
+      <c r="D287" s="375"/>
       <c r="E287" s="359"/>
       <c r="G287" s="31"/>
       <c r="H287" s="25"/>
@@ -42489,7 +42489,7 @@
       </c>
       <c r="H288" s="25"/>
       <c r="I288" s="25"/>
-      <c r="J288" s="374" t="s">
+      <c r="J288" s="378" t="s">
         <v>2543</v>
       </c>
       <c r="L288" s="31"/>
@@ -42510,13 +42510,13 @@
       <c r="G289" s="31"/>
       <c r="H289" s="25"/>
       <c r="I289" s="25"/>
-      <c r="J289" s="375"/>
+      <c r="J289" s="379"/>
       <c r="L289" s="31" t="s">
         <v>2536</v>
       </c>
       <c r="M289" s="25"/>
       <c r="N289" s="25"/>
-      <c r="O289" s="374" t="s">
+      <c r="O289" s="378" t="s">
         <v>2542</v>
       </c>
     </row>
@@ -42525,34 +42525,34 @@
       <c r="C290" s="25"/>
       <c r="D290" s="25"/>
       <c r="E290" s="32"/>
-      <c r="G290" s="373" t="s">
+      <c r="G290" s="377" t="s">
         <v>2544</v>
       </c>
-      <c r="H290" s="371"/>
-      <c r="I290" s="371"/>
-      <c r="J290" s="375"/>
+      <c r="H290" s="375"/>
+      <c r="I290" s="375"/>
+      <c r="J290" s="379"/>
       <c r="L290" s="31"/>
       <c r="M290" s="25"/>
       <c r="N290" s="25"/>
-      <c r="O290" s="375"/>
+      <c r="O290" s="379"/>
     </row>
     <row r="291" spans="2:15">
       <c r="B291" s="360"/>
-      <c r="C291" s="371" t="s">
+      <c r="C291" s="375" t="s">
         <v>2538</v>
       </c>
-      <c r="D291" s="371"/>
+      <c r="D291" s="375"/>
       <c r="E291" s="359"/>
       <c r="G291" s="31"/>
       <c r="H291" s="25"/>
       <c r="I291" s="25"/>
-      <c r="J291" s="375"/>
-      <c r="L291" s="373" t="s">
+      <c r="J291" s="379"/>
+      <c r="L291" s="377" t="s">
         <v>2539</v>
       </c>
-      <c r="M291" s="371"/>
-      <c r="N291" s="371"/>
-      <c r="O291" s="375"/>
+      <c r="M291" s="375"/>
+      <c r="N291" s="375"/>
+      <c r="O291" s="379"/>
     </row>
     <row r="292" spans="2:15">
       <c r="B292" s="31"/>
@@ -42566,7 +42566,7 @@
       <c r="L292" s="31"/>
       <c r="M292" s="25"/>
       <c r="N292" s="25"/>
-      <c r="O292" s="375"/>
+      <c r="O292" s="379"/>
     </row>
     <row r="293" spans="2:15">
       <c r="B293" s="31"/>
@@ -42663,11 +42663,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="H227:I227"/>
-    <mergeCell ref="K227:L227"/>
-    <mergeCell ref="D227:F227"/>
-    <mergeCell ref="D223:F223"/>
-    <mergeCell ref="D273:D278"/>
     <mergeCell ref="C287:E287"/>
     <mergeCell ref="C291:E291"/>
     <mergeCell ref="B287:B291"/>
@@ -42675,6 +42670,11 @@
     <mergeCell ref="O289:O292"/>
     <mergeCell ref="J288:J291"/>
     <mergeCell ref="G290:I290"/>
+    <mergeCell ref="H227:I227"/>
+    <mergeCell ref="K227:L227"/>
+    <mergeCell ref="D227:F227"/>
+    <mergeCell ref="D223:F223"/>
+    <mergeCell ref="D273:D278"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
variable and method call basics
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pc-basics" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4533" uniqueCount="2551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4565" uniqueCount="2558">
   <si>
     <t>USER</t>
   </si>
@@ -8046,6 +8046,27 @@
   </si>
   <si>
     <t>3) p = #abc</t>
+  </si>
+  <si>
+    <t>p.name="mike";</t>
+  </si>
+  <si>
+    <t>p=method2(p);</t>
+  </si>
+  <si>
+    <t>public Person method2(Person p) {</t>
+  </si>
+  <si>
+    <t>return p;</t>
+  </si>
+  <si>
+    <t>method1  p</t>
+  </si>
+  <si>
+    <t>method2 p</t>
+  </si>
+  <si>
+    <t>return #xyz;</t>
   </si>
 </sst>
 </file>
@@ -9451,18 +9472,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9476,6 +9485,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -19314,8 +19335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M234"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20662,11 +20683,175 @@
       <c r="K91" s="195"/>
       <c r="L91" s="337"/>
     </row>
-    <row r="93" spans="1:13">
+    <row r="92" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="93" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A93" s="36" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D93" s="74" t="s">
+        <v>141</v>
+      </c>
+      <c r="E93" s="75" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F93" s="77"/>
+      <c r="G93" s="77"/>
+      <c r="H93" s="77"/>
+      <c r="I93" s="77"/>
+      <c r="J93" s="77"/>
+      <c r="K93" s="78"/>
       <c r="M93" s="259"/>
     </row>
-    <row r="96" spans="1:13">
+    <row r="94" spans="1:13">
+      <c r="B94" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="D94" s="79" t="s">
+        <v>2555</v>
+      </c>
+      <c r="E94" s="36" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H94" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="I94" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="J94" s="78" t="s">
+        <v>343</v>
+      </c>
+      <c r="K94" s="71"/>
+    </row>
+    <row r="95" spans="1:13" ht="15.75" thickBot="1">
+      <c r="B95" s="36" t="s">
+        <v>2551</v>
+      </c>
+      <c r="D95" s="79" t="s">
+        <v>2556</v>
+      </c>
+      <c r="E95" s="36" t="s">
+        <v>1217</v>
+      </c>
+      <c r="I95" s="80"/>
+      <c r="J95" s="82"/>
+      <c r="K95" s="71"/>
+    </row>
+    <row r="96" spans="1:13" ht="15.75" thickBot="1">
+      <c r="B96" s="36" t="s">
+        <v>2552</v>
+      </c>
+      <c r="D96" s="79"/>
       <c r="I96" s="259"/>
+      <c r="K96" s="71"/>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="B97" s="36" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D97" s="79"/>
+      <c r="H97" s="36" t="s">
+        <v>1217</v>
+      </c>
+      <c r="I97" s="76"/>
+      <c r="J97" s="78"/>
+      <c r="K97" s="71"/>
+    </row>
+    <row r="98" spans="1:11" ht="15.75" thickBot="1">
+      <c r="B98" s="36" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D98" s="79" t="s">
+        <v>275</v>
+      </c>
+      <c r="I98" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="J98" s="82" t="s">
+        <v>308</v>
+      </c>
+      <c r="K98" s="71"/>
+    </row>
+    <row r="99" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A99" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D99" s="79"/>
+      <c r="K99" s="71"/>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" s="36" t="s">
+        <v>2553</v>
+      </c>
+      <c r="D100" s="79"/>
+      <c r="H100" s="36" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I100" s="76"/>
+      <c r="J100" s="78"/>
+      <c r="K100" s="71"/>
+    </row>
+    <row r="101" spans="1:11" ht="15.75" thickBot="1">
+      <c r="B101" s="36" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D101" s="79"/>
+      <c r="I101" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="J101" s="82" t="s">
+        <v>275</v>
+      </c>
+      <c r="K101" s="71"/>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="B102" s="36" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C102" s="36" t="s">
+        <v>2557</v>
+      </c>
+      <c r="D102" s="79"/>
+      <c r="K102" s="71"/>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="B103" s="36" t="s">
+        <v>2554</v>
+      </c>
+      <c r="D103" s="79"/>
+      <c r="K103" s="71"/>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D104" s="79"/>
+      <c r="K104" s="71"/>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" s="36" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D105" s="79"/>
+      <c r="K105" s="71"/>
+    </row>
+    <row r="106" spans="1:11" ht="15.75" thickBot="1">
+      <c r="B106" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="D106" s="80"/>
+      <c r="E106" s="81"/>
+      <c r="F106" s="81"/>
+      <c r="G106" s="81"/>
+      <c r="H106" s="81"/>
+      <c r="I106" s="81"/>
+      <c r="J106" s="81"/>
+      <c r="K106" s="82"/>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107" s="36" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="140" spans="5:10">
       <c r="E140" s="324"/>
@@ -37738,11 +37923,11 @@
       <c r="B223" t="s">
         <v>1190</v>
       </c>
-      <c r="D223" s="372" t="s">
+      <c r="D223" s="377" t="s">
         <v>41</v>
       </c>
-      <c r="E223" s="374"/>
-      <c r="F223" s="373"/>
+      <c r="E223" s="379"/>
+      <c r="F223" s="378"/>
       <c r="H223" s="31"/>
       <c r="I223" s="32"/>
       <c r="K223" s="31"/>
@@ -37794,19 +37979,19 @@
       <c r="B227" t="s">
         <v>1413</v>
       </c>
-      <c r="D227" s="372" t="s">
+      <c r="D227" s="377" t="s">
         <v>1212</v>
       </c>
-      <c r="E227" s="374"/>
-      <c r="F227" s="373"/>
-      <c r="H227" s="372" t="s">
+      <c r="E227" s="379"/>
+      <c r="F227" s="378"/>
+      <c r="H227" s="377" t="s">
         <v>1215</v>
       </c>
-      <c r="I227" s="373"/>
-      <c r="K227" s="372" t="s">
+      <c r="I227" s="378"/>
+      <c r="K227" s="377" t="s">
         <v>1214</v>
       </c>
-      <c r="L227" s="373"/>
+      <c r="L227" s="378"/>
     </row>
     <row r="228" spans="2:12">
       <c r="D228" s="31" t="s">
@@ -38053,7 +38238,7 @@
       </c>
     </row>
     <row r="273" spans="2:15">
-      <c r="D273" s="375" t="s">
+      <c r="D273" s="380" t="s">
         <v>1854</v>
       </c>
       <c r="F273" s="137" t="s">
@@ -38061,22 +38246,22 @@
       </c>
     </row>
     <row r="274" spans="2:15">
-      <c r="D274" s="375"/>
+      <c r="D274" s="380"/>
     </row>
     <row r="275" spans="2:15">
-      <c r="D275" s="375"/>
+      <c r="D275" s="380"/>
       <c r="F275" t="s">
         <v>1853</v>
       </c>
     </row>
     <row r="276" spans="2:15">
-      <c r="D276" s="375"/>
+      <c r="D276" s="380"/>
       <c r="K276" t="s">
         <v>1869</v>
       </c>
     </row>
     <row r="277" spans="2:15">
-      <c r="D277" s="375"/>
+      <c r="D277" s="380"/>
       <c r="F277" s="137" t="s">
         <v>1413</v>
       </c>
@@ -38091,7 +38276,7 @@
       </c>
     </row>
     <row r="278" spans="2:15">
-      <c r="D278" s="375"/>
+      <c r="D278" s="380"/>
       <c r="I278" t="s">
         <v>1871</v>
       </c>
@@ -38177,13 +38362,13 @@
       <c r="O286" s="32"/>
     </row>
     <row r="287" spans="2:15">
-      <c r="B287" s="377" t="s">
+      <c r="B287" s="373" t="s">
         <v>1864</v>
       </c>
-      <c r="C287" s="376" t="s">
+      <c r="C287" s="372" t="s">
         <v>1206</v>
       </c>
-      <c r="D287" s="376"/>
+      <c r="D287" s="372"/>
       <c r="E287" s="360"/>
       <c r="G287" s="31"/>
       <c r="H287" s="25"/>
@@ -38206,7 +38391,7 @@
       </c>
       <c r="H288" s="25"/>
       <c r="I288" s="25"/>
-      <c r="J288" s="379" t="s">
+      <c r="J288" s="375" t="s">
         <v>1866</v>
       </c>
       <c r="L288" s="31"/>
@@ -38227,13 +38412,13 @@
       <c r="G289" s="31"/>
       <c r="H289" s="25"/>
       <c r="I289" s="25"/>
-      <c r="J289" s="380"/>
+      <c r="J289" s="376"/>
       <c r="L289" s="31" t="s">
         <v>1859</v>
       </c>
       <c r="M289" s="25"/>
       <c r="N289" s="25"/>
-      <c r="O289" s="379" t="s">
+      <c r="O289" s="375" t="s">
         <v>1865</v>
       </c>
     </row>
@@ -38242,34 +38427,34 @@
       <c r="C290" s="25"/>
       <c r="D290" s="25"/>
       <c r="E290" s="32"/>
-      <c r="G290" s="378" t="s">
+      <c r="G290" s="374" t="s">
         <v>1867</v>
       </c>
-      <c r="H290" s="376"/>
-      <c r="I290" s="376"/>
-      <c r="J290" s="380"/>
+      <c r="H290" s="372"/>
+      <c r="I290" s="372"/>
+      <c r="J290" s="376"/>
       <c r="L290" s="31"/>
       <c r="M290" s="25"/>
       <c r="N290" s="25"/>
-      <c r="O290" s="380"/>
+      <c r="O290" s="376"/>
     </row>
     <row r="291" spans="2:15">
       <c r="B291" s="361"/>
-      <c r="C291" s="376" t="s">
+      <c r="C291" s="372" t="s">
         <v>1861</v>
       </c>
-      <c r="D291" s="376"/>
+      <c r="D291" s="372"/>
       <c r="E291" s="360"/>
       <c r="G291" s="31"/>
       <c r="H291" s="25"/>
       <c r="I291" s="25"/>
-      <c r="J291" s="380"/>
-      <c r="L291" s="378" t="s">
+      <c r="J291" s="376"/>
+      <c r="L291" s="374" t="s">
         <v>1862</v>
       </c>
-      <c r="M291" s="376"/>
-      <c r="N291" s="376"/>
-      <c r="O291" s="380"/>
+      <c r="M291" s="372"/>
+      <c r="N291" s="372"/>
+      <c r="O291" s="376"/>
     </row>
     <row r="292" spans="2:15">
       <c r="B292" s="31"/>
@@ -38283,7 +38468,7 @@
       <c r="L292" s="31"/>
       <c r="M292" s="25"/>
       <c r="N292" s="25"/>
-      <c r="O292" s="380"/>
+      <c r="O292" s="376"/>
     </row>
     <row r="293" spans="2:15">
       <c r="B293" s="31"/>
@@ -38533,6 +38718,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="H227:I227"/>
+    <mergeCell ref="K227:L227"/>
+    <mergeCell ref="D227:F227"/>
+    <mergeCell ref="D223:F223"/>
+    <mergeCell ref="D273:D278"/>
     <mergeCell ref="C287:E287"/>
     <mergeCell ref="C291:E291"/>
     <mergeCell ref="B287:B291"/>
@@ -38540,11 +38730,6 @@
     <mergeCell ref="O289:O292"/>
     <mergeCell ref="J288:J291"/>
     <mergeCell ref="G290:I290"/>
-    <mergeCell ref="H227:I227"/>
-    <mergeCell ref="K227:L227"/>
-    <mergeCell ref="D227:F227"/>
-    <mergeCell ref="D223:F223"/>
-    <mergeCell ref="D273:D278"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -41236,7 +41421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A75" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
operators and variabel scope
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4756" uniqueCount="2538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2540">
   <si>
     <t>USER</t>
   </si>
@@ -8076,6 +8076,12 @@
   </si>
   <si>
     <t>garbage collection</t>
+  </si>
+  <si>
+    <t>21/10</t>
+  </si>
+  <si>
+    <t>21%10</t>
   </si>
 </sst>
 </file>
@@ -9589,6 +9595,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9659,10 +9683,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -9710,24 +9734,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10084,13 +10090,13 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="15.75" thickBot="1">
-      <c r="H3" s="428" t="s">
+      <c r="H3" s="436" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="429"/>
-      <c r="J3" s="429"/>
-      <c r="K3" s="429"/>
-      <c r="L3" s="430"/>
+      <c r="I3" s="437"/>
+      <c r="J3" s="437"/>
+      <c r="K3" s="437"/>
+      <c r="L3" s="438"/>
       <c r="Q3" t="s">
         <v>2362</v>
       </c>
@@ -10122,20 +10128,20 @@
       <c r="F6" s="4" t="s">
         <v>1675</v>
       </c>
-      <c r="G6" s="431" t="s">
+      <c r="G6" s="439" t="s">
         <v>1189</v>
       </c>
-      <c r="H6" s="432"/>
+      <c r="H6" s="440"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="431" t="s">
+      <c r="J6" s="439" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="432"/>
+      <c r="K6" s="440"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="431" t="s">
+      <c r="M6" s="439" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="432"/>
+      <c r="N6" s="440"/>
       <c r="P6" t="s">
         <v>2354</v>
       </c>
@@ -10169,20 +10175,20 @@
       <c r="F8" s="4" t="s">
         <v>1216</v>
       </c>
-      <c r="G8" s="433" t="s">
+      <c r="G8" s="441" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="434"/>
+      <c r="H8" s="442"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="433" t="s">
+      <c r="J8" s="441" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="434"/>
+      <c r="K8" s="442"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="433" t="s">
+      <c r="M8" s="441" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="434"/>
+      <c r="N8" s="442"/>
       <c r="P8" t="s">
         <v>2356</v>
       </c>
@@ -10208,29 +10214,29 @@
       <c r="Q9" s="119"/>
     </row>
     <row r="10" spans="2:18">
-      <c r="F10" s="424" t="s">
+      <c r="F10" s="432" t="s">
         <v>1687</v>
       </c>
-      <c r="G10" s="425"/>
-      <c r="H10" s="425"/>
-      <c r="I10" s="425"/>
-      <c r="J10" s="425"/>
-      <c r="K10" s="425"/>
-      <c r="L10" s="425"/>
-      <c r="M10" s="425"/>
-      <c r="N10" s="425"/>
+      <c r="G10" s="433"/>
+      <c r="H10" s="433"/>
+      <c r="I10" s="433"/>
+      <c r="J10" s="433"/>
+      <c r="K10" s="433"/>
+      <c r="L10" s="433"/>
+      <c r="M10" s="433"/>
+      <c r="N10" s="433"/>
       <c r="Q10" s="119"/>
     </row>
     <row r="11" spans="2:18" ht="15.75" thickBot="1">
-      <c r="F11" s="426"/>
-      <c r="G11" s="427"/>
-      <c r="H11" s="427"/>
-      <c r="I11" s="427"/>
-      <c r="J11" s="427"/>
-      <c r="K11" s="427"/>
-      <c r="L11" s="427"/>
-      <c r="M11" s="427"/>
-      <c r="N11" s="427"/>
+      <c r="F11" s="434"/>
+      <c r="G11" s="435"/>
+      <c r="H11" s="435"/>
+      <c r="I11" s="435"/>
+      <c r="J11" s="435"/>
+      <c r="K11" s="435"/>
+      <c r="L11" s="435"/>
+      <c r="M11" s="435"/>
+      <c r="N11" s="435"/>
     </row>
     <row r="12" spans="2:18">
       <c r="D12" s="103" t="s">
@@ -10478,8 +10484,8 @@
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75" thickBot="1">
-      <c r="D23" s="422"/>
-      <c r="E23" s="423"/>
+      <c r="D23" s="430"/>
+      <c r="E23" s="431"/>
       <c r="F23" s="118"/>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
@@ -21152,34 +21158,34 @@
       <c r="E10" t="s">
         <v>1880</v>
       </c>
-      <c r="G10" s="435" t="s">
+      <c r="G10" s="443" t="s">
         <v>1887</v>
       </c>
-      <c r="H10" s="436"/>
-      <c r="I10" s="437"/>
+      <c r="H10" s="444"/>
+      <c r="I10" s="445"/>
       <c r="K10" s="28" t="s">
         <v>1897</v>
       </c>
       <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="G11" s="438"/>
-      <c r="H11" s="439"/>
-      <c r="I11" s="440"/>
+      <c r="G11" s="446"/>
+      <c r="H11" s="447"/>
+      <c r="I11" s="448"/>
       <c r="K11" s="31"/>
       <c r="L11" s="32"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1">
-      <c r="G12" s="438"/>
-      <c r="H12" s="439"/>
-      <c r="I12" s="440"/>
+      <c r="G12" s="446"/>
+      <c r="H12" s="447"/>
+      <c r="I12" s="448"/>
       <c r="K12" s="33"/>
       <c r="L12" s="35"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1">
-      <c r="G13" s="441"/>
-      <c r="H13" s="442"/>
-      <c r="I13" s="443"/>
+      <c r="G13" s="449"/>
+      <c r="H13" s="450"/>
+      <c r="I13" s="451"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1">
       <c r="E14" t="s">
@@ -22108,7 +22114,7 @@
       </c>
       <c r="J3" s="83"/>
       <c r="K3" s="279"/>
-      <c r="L3" s="449" t="s">
+      <c r="L3" s="457" t="s">
         <v>1498</v>
       </c>
       <c r="M3" s="170"/>
@@ -22130,7 +22136,7 @@
       <c r="K4" s="69">
         <v>123</v>
       </c>
-      <c r="L4" s="450"/>
+      <c r="L4" s="458"/>
       <c r="M4" s="170"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
@@ -22150,12 +22156,12 @@
       <c r="K5" s="280" t="s">
         <v>1497</v>
       </c>
-      <c r="L5" s="450"/>
+      <c r="L5" s="458"/>
       <c r="M5" s="170"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1">
       <c r="F6" s="187"/>
-      <c r="L6" s="450"/>
+      <c r="L6" s="458"/>
       <c r="M6" s="170"/>
     </row>
     <row r="7" spans="1:13">
@@ -22168,7 +22174,7 @@
       </c>
       <c r="J7" s="83"/>
       <c r="K7" s="279"/>
-      <c r="L7" s="450"/>
+      <c r="L7" s="458"/>
       <c r="M7" s="170"/>
     </row>
     <row r="8" spans="1:13">
@@ -22186,7 +22192,7 @@
       <c r="K8" s="69">
         <v>111</v>
       </c>
-      <c r="L8" s="450"/>
+      <c r="L8" s="458"/>
       <c r="M8" s="170"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1">
@@ -22200,7 +22206,7 @@
       <c r="K9" s="263" t="s">
         <v>164</v>
       </c>
-      <c r="L9" s="450"/>
+      <c r="L9" s="458"/>
       <c r="M9" s="170"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1">
@@ -22208,7 +22214,7 @@
         <v>1481</v>
       </c>
       <c r="F10" s="187"/>
-      <c r="L10" s="450"/>
+      <c r="L10" s="458"/>
       <c r="M10" s="170"/>
     </row>
     <row r="11" spans="1:13">
@@ -22221,7 +22227,7 @@
       </c>
       <c r="J11" s="83"/>
       <c r="K11" s="279"/>
-      <c r="L11" s="450"/>
+      <c r="L11" s="458"/>
       <c r="M11" s="170"/>
     </row>
     <row r="12" spans="1:13">
@@ -22235,7 +22241,7 @@
       <c r="K12" s="69">
         <v>222</v>
       </c>
-      <c r="L12" s="450"/>
+      <c r="L12" s="458"/>
       <c r="M12" s="170"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1">
@@ -22252,7 +22258,7 @@
       <c r="K13" s="263" t="s">
         <v>199</v>
       </c>
-      <c r="L13" s="451"/>
+      <c r="L13" s="459"/>
       <c r="M13" s="170"/>
     </row>
     <row r="14" spans="1:13">
@@ -22274,10 +22280,10 @@
       <c r="D15" s="258"/>
       <c r="E15" s="258"/>
       <c r="F15" s="187"/>
-      <c r="J15" s="444" t="s">
+      <c r="J15" s="452" t="s">
         <v>1487</v>
       </c>
-      <c r="K15" s="444"/>
+      <c r="K15" s="452"/>
       <c r="L15" s="69" t="s">
         <v>539</v>
       </c>
@@ -22297,8 +22303,8 @@
       <c r="G16" s="96" t="s">
         <v>1489</v>
       </c>
-      <c r="J16" s="444"/>
-      <c r="K16" s="444"/>
+      <c r="J16" s="452"/>
+      <c r="K16" s="452"/>
       <c r="L16" s="69" t="s">
         <v>50</v>
       </c>
@@ -22376,48 +22382,48 @@
     <row r="22" spans="1:13">
       <c r="A22" s="96"/>
       <c r="B22" s="96"/>
-      <c r="K22" s="446"/>
+      <c r="K22" s="453"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="96"/>
       <c r="B23" s="96"/>
-      <c r="K23" s="445"/>
+      <c r="K23" s="454"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="96"/>
       <c r="B24" s="96"/>
-      <c r="K24" s="445"/>
+      <c r="K24" s="454"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="96"/>
       <c r="B25" s="96"/>
-      <c r="K25" s="445"/>
+      <c r="K25" s="454"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="96"/>
       <c r="B26" s="96"/>
-      <c r="K26" s="445"/>
+      <c r="K26" s="454"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="K27" s="445"/>
+      <c r="K27" s="454"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="K28" s="445"/>
+      <c r="K28" s="454"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="96"/>
-      <c r="K29" s="445"/>
+      <c r="K29" s="454"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="96"/>
-      <c r="K30" s="445"/>
+      <c r="K30" s="454"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="96"/>
-      <c r="K31" s="445"/>
+      <c r="K31" s="454"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="K32" s="445"/>
+      <c r="K32" s="454"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="276"/>
@@ -30901,18 +30907,18 @@
       </c>
     </row>
     <row r="8" spans="1:38">
-      <c r="B8" s="453" t="s">
+      <c r="B8" s="461" t="s">
         <v>1629</v>
       </c>
-      <c r="C8" s="453"/>
-      <c r="F8" s="453" t="s">
+      <c r="C8" s="461"/>
+      <c r="F8" s="461" t="s">
         <v>1630</v>
       </c>
-      <c r="G8" s="453"/>
-      <c r="I8" s="453" t="s">
+      <c r="G8" s="461"/>
+      <c r="I8" s="461" t="s">
         <v>1630</v>
       </c>
-      <c r="J8" s="453"/>
+      <c r="J8" s="461"/>
       <c r="M8" s="108"/>
       <c r="N8" s="39"/>
       <c r="R8" t="b">
@@ -30935,18 +30941,18 @@
       </c>
     </row>
     <row r="9" spans="1:38">
-      <c r="F9" s="454" t="s">
+      <c r="F9" s="462" t="s">
         <v>1631</v>
       </c>
-      <c r="G9" s="454"/>
-      <c r="I9" s="454" t="s">
+      <c r="G9" s="462"/>
+      <c r="I9" s="462" t="s">
         <v>1265</v>
       </c>
-      <c r="J9" s="454"/>
-      <c r="M9" s="455" t="s">
+      <c r="J9" s="462"/>
+      <c r="M9" s="463" t="s">
         <v>1630</v>
       </c>
-      <c r="N9" s="455"/>
+      <c r="N9" s="463"/>
       <c r="AA9">
         <v>1000000</v>
       </c>
@@ -30994,19 +31000,19 @@
       </c>
     </row>
     <row r="11" spans="1:38">
-      <c r="E11" s="452" t="s">
+      <c r="E11" s="460" t="s">
         <v>1633</v>
       </c>
-      <c r="F11" s="452"/>
-      <c r="G11" s="452"/>
-      <c r="H11" s="452"/>
-      <c r="I11" s="452"/>
-      <c r="J11" s="452"/>
-      <c r="K11" s="452"/>
-      <c r="L11" s="452"/>
-      <c r="M11" s="452"/>
-      <c r="N11" s="452"/>
-      <c r="O11" s="452"/>
+      <c r="F11" s="460"/>
+      <c r="G11" s="460"/>
+      <c r="H11" s="460"/>
+      <c r="I11" s="460"/>
+      <c r="J11" s="460"/>
+      <c r="K11" s="460"/>
+      <c r="L11" s="460"/>
+      <c r="M11" s="460"/>
+      <c r="N11" s="460"/>
+      <c r="O11" s="460"/>
       <c r="R11" t="s">
         <v>1870</v>
       </c>
@@ -34553,10 +34559,10 @@
       </c>
     </row>
     <row r="241" spans="1:12">
-      <c r="C241" s="422" t="s">
+      <c r="C241" s="430" t="s">
         <v>1657</v>
       </c>
-      <c r="D241" s="422"/>
+      <c r="D241" s="430"/>
       <c r="E241" s="122" t="s">
         <v>30</v>
       </c>
@@ -35095,10 +35101,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:21">
-      <c r="C2" s="456" t="s">
+      <c r="C2" s="464" t="s">
         <v>1328</v>
       </c>
-      <c r="D2" s="456"/>
+      <c r="D2" s="464"/>
       <c r="F2" s="25" t="s">
         <v>2338</v>
       </c>
@@ -36172,10 +36178,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M234"/>
+  <dimension ref="A1:S234"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55:H57"/>
+    <sheetView tabSelected="1" topLeftCell="M23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36475,12 +36481,12 @@
       <c r="L16" s="302"/>
       <c r="M16" s="302"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:19">
       <c r="A17" s="36" t="s">
         <v>2459</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1">
+    <row r="18" spans="1:19" ht="15.75" thickBot="1">
       <c r="A18" s="257" t="s">
         <v>1704</v>
       </c>
@@ -36488,7 +36494,7 @@
         <v>2444</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1">
+    <row r="19" spans="1:19" ht="15.75" thickBot="1">
       <c r="B19" s="36" t="s">
         <v>137</v>
       </c>
@@ -36505,7 +36511,7 @@
       <c r="J19" s="76"/>
       <c r="K19" s="77"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:19">
       <c r="B20" s="36" t="s">
         <v>2439</v>
       </c>
@@ -36527,7 +36533,7 @@
       </c>
       <c r="K20" s="70"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1">
+    <row r="21" spans="1:19" ht="15.75" thickBot="1">
       <c r="A21" s="36" t="s">
         <v>37</v>
       </c>
@@ -36549,7 +36555,7 @@
       <c r="K21" s="170"/>
       <c r="L21" s="421"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+    <row r="22" spans="1:19" ht="15.75" thickBot="1">
       <c r="A22" s="36" t="s">
         <v>2443</v>
       </c>
@@ -36567,7 +36573,7 @@
       <c r="K22" s="170"/>
       <c r="L22" s="421"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:19">
       <c r="A23" s="36" t="s">
         <v>92</v>
       </c>
@@ -36591,7 +36597,7 @@
       <c r="K23" s="170"/>
       <c r="L23" s="421"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1">
+    <row r="24" spans="1:19" ht="15.75" thickBot="1">
       <c r="A24" s="36" t="s">
         <v>2440</v>
       </c>
@@ -36607,7 +36613,7 @@
       </c>
       <c r="K24" s="70"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:19">
       <c r="A25" s="36" t="s">
         <v>2441</v>
       </c>
@@ -36619,8 +36625,14 @@
       <c r="J25" s="421"/>
       <c r="K25" s="170"/>
       <c r="L25" s="421"/>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="R25" s="36" t="s">
+        <v>2538</v>
+      </c>
+      <c r="S25" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="36" t="s">
         <v>2442</v>
       </c>
@@ -36633,8 +36645,14 @@
       <c r="J26" s="421"/>
       <c r="K26" s="170"/>
       <c r="L26" s="421"/>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="R26" s="36" t="s">
+        <v>2539</v>
+      </c>
+      <c r="S26" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="D27" s="78"/>
       <c r="F27" s="421"/>
       <c r="G27" s="96"/>
@@ -36644,7 +36662,7 @@
       <c r="K27" s="170"/>
       <c r="L27" s="421"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:19">
       <c r="A28" s="36" t="s">
         <v>2454</v>
       </c>
@@ -36657,8 +36675,11 @@
       <c r="J28" s="421"/>
       <c r="K28" s="170"/>
       <c r="L28" s="421"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="R28" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="36" t="s">
         <v>2456</v>
       </c>
@@ -36671,8 +36692,14 @@
       <c r="J29" s="421"/>
       <c r="K29" s="170"/>
       <c r="L29" s="421"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="Q29" s="36">
+        <v>10</v>
+      </c>
+      <c r="R29" s="36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="36" t="s">
         <v>2460</v>
       </c>
@@ -36688,8 +36715,11 @@
       <c r="J30" s="421"/>
       <c r="K30" s="170"/>
       <c r="L30" s="421"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="R30" s="36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="36" t="s">
         <v>2462</v>
       </c>
@@ -36705,8 +36735,11 @@
       <c r="J31" s="421"/>
       <c r="K31" s="170"/>
       <c r="L31" s="421"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="R31" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="36" t="s">
         <v>2463</v>
       </c>
@@ -37149,7 +37182,7 @@
       <c r="E63" s="96"/>
       <c r="F63" s="421"/>
       <c r="G63" s="106"/>
-      <c r="H63" s="463" t="s">
+      <c r="H63" s="422" t="s">
         <v>2490</v>
       </c>
       <c r="I63" s="96"/>
@@ -37177,15 +37210,15 @@
       </c>
       <c r="D65" s="315"/>
       <c r="E65" s="96"/>
-      <c r="F65" s="464" t="s">
+      <c r="F65" s="423" t="s">
         <v>2485</v>
       </c>
       <c r="G65" s="421"/>
-      <c r="H65" s="464" t="s">
+      <c r="H65" s="423" t="s">
         <v>2487</v>
       </c>
       <c r="I65" s="421"/>
-      <c r="J65" s="464" t="s">
+      <c r="J65" s="423" t="s">
         <v>2486</v>
       </c>
       <c r="K65" s="170"/>
@@ -37909,7 +37942,7 @@
       <c r="E119" s="421"/>
       <c r="F119" s="96"/>
       <c r="G119" s="421"/>
-      <c r="H119" s="468" t="s">
+      <c r="H119" s="427" t="s">
         <v>2450</v>
       </c>
       <c r="I119" s="83" t="s">
@@ -37935,7 +37968,7 @@
       <c r="K120" s="70"/>
     </row>
     <row r="121" spans="1:12" ht="15.75" thickBot="1">
-      <c r="D121" s="469" t="s">
+      <c r="D121" s="428" t="s">
         <v>2530</v>
       </c>
       <c r="E121" s="83" t="s">
@@ -37960,7 +37993,7 @@
       <c r="E122" s="188"/>
       <c r="F122" s="189"/>
       <c r="G122" s="421"/>
-      <c r="H122" s="470" t="s">
+      <c r="H122" s="429" t="s">
         <v>2528</v>
       </c>
       <c r="I122" s="83" t="s">
@@ -37992,7 +38025,7 @@
       <c r="B124" s="36" t="s">
         <v>2527</v>
       </c>
-      <c r="D124" s="469" t="s">
+      <c r="D124" s="428" t="s">
         <v>2531</v>
       </c>
       <c r="E124" s="83" t="s">
@@ -38013,7 +38046,7 @@
       <c r="E125" s="188"/>
       <c r="F125" s="189"/>
       <c r="G125" s="421"/>
-      <c r="H125" s="470" t="s">
+      <c r="H125" s="429" t="s">
         <v>2529</v>
       </c>
       <c r="I125" s="83" t="s">
@@ -38039,7 +38072,7 @@
       <c r="L126" s="421"/>
     </row>
     <row r="127" spans="1:12">
-      <c r="D127" s="469" t="s">
+      <c r="D127" s="428" t="s">
         <v>2532</v>
       </c>
       <c r="E127" s="83" t="s">
@@ -38214,7 +38247,7 @@
         <v>2502</v>
       </c>
       <c r="H158" s="136"/>
-      <c r="I158" s="465"/>
+      <c r="I158" s="424"/>
       <c r="J158" s="377"/>
       <c r="L158" s="136"/>
     </row>
@@ -38239,7 +38272,7 @@
       <c r="E161" s="286" t="s">
         <v>2500</v>
       </c>
-      <c r="F161" s="465"/>
+      <c r="F161" s="424"/>
       <c r="G161" s="136"/>
       <c r="I161" s="377"/>
       <c r="J161" s="286" t="s">
@@ -38252,7 +38285,7 @@
       <c r="D162" s="258"/>
       <c r="E162" s="377"/>
       <c r="F162" s="377"/>
-      <c r="G162" s="466"/>
+      <c r="G162" s="425"/>
       <c r="I162" s="377"/>
       <c r="J162" s="377"/>
     </row>
@@ -38260,7 +38293,7 @@
       <c r="D163" s="258"/>
       <c r="E163" s="377"/>
       <c r="F163" s="377"/>
-      <c r="G163" s="466"/>
+      <c r="G163" s="425"/>
     </row>
     <row r="164" spans="3:12">
       <c r="D164" s="258"/>
@@ -38315,30 +38348,30 @@
       <c r="E169" s="421" t="s">
         <v>2504</v>
       </c>
-      <c r="F169" s="467" t="s">
+      <c r="F169" s="426" t="s">
         <v>2101</v>
       </c>
-      <c r="G169" s="466"/>
+      <c r="G169" s="425"/>
       <c r="H169" s="36" t="s">
         <v>2505</v>
       </c>
-      <c r="I169" s="466" t="s">
+      <c r="I169" s="425" t="s">
         <v>2509</v>
       </c>
-      <c r="J169" s="466"/>
+      <c r="J169" s="425"/>
       <c r="K169" s="36" t="s">
         <v>2508</v>
       </c>
     </row>
     <row r="170" spans="3:12">
       <c r="D170" s="258"/>
-      <c r="E170" s="466" t="s">
+      <c r="E170" s="425" t="s">
         <v>2512</v>
       </c>
       <c r="F170" s="421"/>
     </row>
     <row r="171" spans="3:12">
-      <c r="E171" s="466" t="s">
+      <c r="E171" s="425" t="s">
         <v>2512</v>
       </c>
       <c r="F171" s="421"/>
@@ -38347,10 +38380,10 @@
       <c r="C172" s="36" t="s">
         <v>2492</v>
       </c>
-      <c r="D172" s="466" t="s">
+      <c r="D172" s="425" t="s">
         <v>2509</v>
       </c>
-      <c r="E172" s="466"/>
+      <c r="E172" s="425"/>
       <c r="F172" s="36" t="s">
         <v>2513</v>
       </c>
@@ -38754,10 +38787,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="2:13">
-      <c r="B1" s="457" t="s">
+      <c r="B1" s="465" t="s">
         <v>1328</v>
       </c>
-      <c r="C1" s="457"/>
+      <c r="C1" s="465"/>
       <c r="E1" t="s">
         <v>1329</v>
       </c>
@@ -40179,18 +40212,18 @@
   <sheetData>
     <row r="2" spans="2:17" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:17" ht="15.75" thickBot="1">
-      <c r="B3" s="458" t="s">
+      <c r="B3" s="466" t="s">
         <v>1353</v>
       </c>
-      <c r="C3" s="459"/>
-      <c r="D3" s="459"/>
-      <c r="E3" s="459"/>
-      <c r="F3" s="459"/>
-      <c r="G3" s="459"/>
-      <c r="H3" s="459"/>
-      <c r="I3" s="459"/>
-      <c r="J3" s="459"/>
-      <c r="K3" s="460"/>
+      <c r="C3" s="467"/>
+      <c r="D3" s="467"/>
+      <c r="E3" s="467"/>
+      <c r="F3" s="467"/>
+      <c r="G3" s="467"/>
+      <c r="H3" s="467"/>
+      <c r="I3" s="467"/>
+      <c r="J3" s="467"/>
+      <c r="K3" s="468"/>
     </row>
     <row r="4" spans="2:17" ht="15.75" thickBot="1">
       <c r="G4" t="s">
@@ -40305,24 +40338,24 @@
       <c r="L12" s="25"/>
     </row>
     <row r="15" spans="2:17">
-      <c r="B15" s="461" t="s">
+      <c r="B15" s="469" t="s">
         <v>1354</v>
       </c>
-      <c r="C15" s="462"/>
-      <c r="D15" s="462"/>
-      <c r="E15" s="462"/>
-      <c r="F15" s="462"/>
-      <c r="G15" s="462"/>
-      <c r="H15" s="462"/>
-      <c r="I15" s="462"/>
-      <c r="J15" s="462"/>
-      <c r="K15" s="462"/>
-      <c r="L15" s="462"/>
-      <c r="M15" s="462"/>
-      <c r="N15" s="462"/>
-      <c r="O15" s="462"/>
-      <c r="P15" s="462"/>
-      <c r="Q15" s="462"/>
+      <c r="C15" s="470"/>
+      <c r="D15" s="470"/>
+      <c r="E15" s="470"/>
+      <c r="F15" s="470"/>
+      <c r="G15" s="470"/>
+      <c r="H15" s="470"/>
+      <c r="I15" s="470"/>
+      <c r="J15" s="470"/>
+      <c r="K15" s="470"/>
+      <c r="L15" s="470"/>
+      <c r="M15" s="470"/>
+      <c r="N15" s="470"/>
+      <c r="O15" s="470"/>
+      <c r="P15" s="470"/>
+      <c r="Q15" s="470"/>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1"/>
     <row r="17" spans="1:17">
@@ -41324,75 +41357,80 @@
       <c r="M214" s="367"/>
     </row>
     <row r="223" spans="4:13">
-      <c r="D223" s="444"/>
-      <c r="E223" s="444"/>
+      <c r="D223" s="452"/>
+      <c r="E223" s="452"/>
     </row>
     <row r="227" spans="4:11">
-      <c r="D227" s="444"/>
-      <c r="E227" s="444"/>
-      <c r="G227" s="444"/>
-      <c r="H227" s="444"/>
-      <c r="J227" s="444"/>
-      <c r="K227" s="444"/>
+      <c r="D227" s="452"/>
+      <c r="E227" s="452"/>
+      <c r="G227" s="452"/>
+      <c r="H227" s="452"/>
+      <c r="J227" s="452"/>
+      <c r="K227" s="452"/>
     </row>
     <row r="273" spans="2:9">
-      <c r="D273" s="445"/>
+      <c r="D273" s="454"/>
     </row>
     <row r="274" spans="2:9">
-      <c r="D274" s="445"/>
+      <c r="D274" s="454"/>
     </row>
     <row r="275" spans="2:9">
-      <c r="D275" s="445"/>
+      <c r="D275" s="454"/>
     </row>
     <row r="276" spans="2:9">
-      <c r="D276" s="445"/>
+      <c r="D276" s="454"/>
     </row>
     <row r="277" spans="2:9">
-      <c r="D277" s="445"/>
+      <c r="D277" s="454"/>
     </row>
     <row r="278" spans="2:9">
-      <c r="D278" s="445"/>
+      <c r="D278" s="454"/>
     </row>
     <row r="287" spans="2:9">
-      <c r="B287" s="446"/>
-      <c r="C287" s="444"/>
-      <c r="D287" s="444"/>
+      <c r="B287" s="453"/>
+      <c r="C287" s="452"/>
+      <c r="D287" s="452"/>
     </row>
     <row r="288" spans="2:9">
-      <c r="B288" s="445"/>
-      <c r="I288" s="446"/>
+      <c r="B288" s="454"/>
+      <c r="I288" s="453"/>
     </row>
     <row r="289" spans="2:14">
-      <c r="B289" s="445"/>
-      <c r="I289" s="445"/>
-      <c r="N289" s="446"/>
+      <c r="B289" s="454"/>
+      <c r="I289" s="454"/>
+      <c r="N289" s="453"/>
     </row>
     <row r="290" spans="2:14">
-      <c r="B290" s="445"/>
-      <c r="F290" s="444"/>
-      <c r="G290" s="444"/>
-      <c r="H290" s="444"/>
-      <c r="I290" s="445"/>
-      <c r="N290" s="445"/>
+      <c r="B290" s="454"/>
+      <c r="F290" s="452"/>
+      <c r="G290" s="452"/>
+      <c r="H290" s="452"/>
+      <c r="I290" s="454"/>
+      <c r="N290" s="454"/>
     </row>
     <row r="291" spans="2:14">
-      <c r="B291" s="445"/>
-      <c r="C291" s="444"/>
-      <c r="D291" s="444"/>
-      <c r="I291" s="445"/>
-      <c r="K291" s="444"/>
-      <c r="L291" s="444"/>
-      <c r="M291" s="444"/>
-      <c r="N291" s="445"/>
+      <c r="B291" s="454"/>
+      <c r="C291" s="452"/>
+      <c r="D291" s="452"/>
+      <c r="I291" s="454"/>
+      <c r="K291" s="452"/>
+      <c r="L291" s="452"/>
+      <c r="M291" s="452"/>
+      <c r="N291" s="454"/>
     </row>
     <row r="292" spans="2:14">
-      <c r="N292" s="445"/>
+      <c r="N292" s="454"/>
     </row>
     <row r="306" spans="6:6">
       <c r="F306" s="253"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G227:H227"/>
+    <mergeCell ref="J227:K227"/>
+    <mergeCell ref="D227:E227"/>
+    <mergeCell ref="D223:E223"/>
+    <mergeCell ref="D273:D278"/>
     <mergeCell ref="C287:D287"/>
     <mergeCell ref="C291:D291"/>
     <mergeCell ref="B287:B291"/>
@@ -41400,11 +41438,6 @@
     <mergeCell ref="N289:N292"/>
     <mergeCell ref="I288:I291"/>
     <mergeCell ref="F290:H290"/>
-    <mergeCell ref="G227:H227"/>
-    <mergeCell ref="J227:K227"/>
-    <mergeCell ref="D227:E227"/>
-    <mergeCell ref="D223:E223"/>
-    <mergeCell ref="D273:D278"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -44140,23 +44173,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="448" t="s">
+      <c r="A1" s="456" t="s">
         <v>1107</v>
       </c>
-      <c r="B1" s="448"/>
-      <c r="C1" s="448"/>
-      <c r="D1" s="448"/>
-      <c r="E1" s="448"/>
-      <c r="F1" s="448"/>
-      <c r="I1" s="448" t="s">
+      <c r="B1" s="456"/>
+      <c r="C1" s="456"/>
+      <c r="D1" s="456"/>
+      <c r="E1" s="456"/>
+      <c r="F1" s="456"/>
+      <c r="I1" s="456" t="s">
         <v>1117</v>
       </c>
-      <c r="J1" s="448"/>
-      <c r="K1" s="448"/>
-      <c r="L1" s="448"/>
-      <c r="M1" s="448"/>
-      <c r="N1" s="448"/>
-      <c r="O1" s="448"/>
+      <c r="J1" s="456"/>
+      <c r="K1" s="456"/>
+      <c r="L1" s="456"/>
+      <c r="M1" s="456"/>
+      <c r="N1" s="456"/>
+      <c r="O1" s="456"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -44306,28 +44339,28 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A12" s="431" t="s">
+      <c r="A12" s="439" t="s">
         <v>1119</v>
       </c>
-      <c r="B12" s="447"/>
-      <c r="C12" s="447"/>
-      <c r="D12" s="447"/>
-      <c r="E12" s="447"/>
-      <c r="F12" s="447"/>
-      <c r="G12" s="447"/>
-      <c r="H12" s="432"/>
-      <c r="I12" s="431" t="s">
+      <c r="B12" s="455"/>
+      <c r="C12" s="455"/>
+      <c r="D12" s="455"/>
+      <c r="E12" s="455"/>
+      <c r="F12" s="455"/>
+      <c r="G12" s="455"/>
+      <c r="H12" s="440"/>
+      <c r="I12" s="439" t="s">
         <v>1119</v>
       </c>
-      <c r="J12" s="447"/>
-      <c r="K12" s="447"/>
-      <c r="L12" s="447"/>
-      <c r="M12" s="447"/>
-      <c r="N12" s="447"/>
-      <c r="O12" s="447"/>
-      <c r="P12" s="447"/>
-      <c r="Q12" s="447"/>
-      <c r="R12" s="432"/>
+      <c r="J12" s="455"/>
+      <c r="K12" s="455"/>
+      <c r="L12" s="455"/>
+      <c r="M12" s="455"/>
+      <c r="N12" s="455"/>
+      <c r="O12" s="455"/>
+      <c r="P12" s="455"/>
+      <c r="Q12" s="455"/>
+      <c r="R12" s="440"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="28" t="s">
@@ -44555,14 +44588,14 @@
       <c r="R21" s="35"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="448" t="s">
+      <c r="A24" s="456" t="s">
         <v>1107</v>
       </c>
-      <c r="B24" s="448"/>
-      <c r="C24" s="448"/>
-      <c r="D24" s="448"/>
-      <c r="E24" s="448"/>
-      <c r="F24" s="448"/>
+      <c r="B24" s="456"/>
+      <c r="C24" s="456"/>
+      <c r="D24" s="456"/>
+      <c r="E24" s="456"/>
+      <c r="F24" s="456"/>
       <c r="H24" s="195" t="s">
         <v>1117</v>
       </c>
@@ -44572,11 +44605,11 @@
       <c r="L24" s="195"/>
       <c r="M24" s="195"/>
       <c r="N24" s="195"/>
-      <c r="P24" s="448" t="s">
+      <c r="P24" s="456" t="s">
         <v>1155</v>
       </c>
-      <c r="Q24" s="448"/>
-      <c r="R24" s="448"/>
+      <c r="Q24" s="456"/>
+      <c r="R24" s="456"/>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="86" t="s">
@@ -44816,28 +44849,28 @@
       </c>
     </row>
     <row r="35" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A35" s="431" t="s">
+      <c r="A35" s="439" t="s">
         <v>1156</v>
       </c>
-      <c r="B35" s="447"/>
-      <c r="C35" s="447"/>
-      <c r="D35" s="447"/>
-      <c r="E35" s="447"/>
-      <c r="F35" s="447"/>
-      <c r="G35" s="447"/>
-      <c r="H35" s="432"/>
-      <c r="I35" s="431" t="s">
+      <c r="B35" s="455"/>
+      <c r="C35" s="455"/>
+      <c r="D35" s="455"/>
+      <c r="E35" s="455"/>
+      <c r="F35" s="455"/>
+      <c r="G35" s="455"/>
+      <c r="H35" s="440"/>
+      <c r="I35" s="439" t="s">
         <v>543</v>
       </c>
-      <c r="J35" s="447"/>
-      <c r="K35" s="447"/>
-      <c r="L35" s="447"/>
-      <c r="M35" s="447"/>
-      <c r="N35" s="447"/>
-      <c r="O35" s="447"/>
-      <c r="P35" s="447"/>
-      <c r="Q35" s="447"/>
-      <c r="R35" s="432"/>
+      <c r="J35" s="455"/>
+      <c r="K35" s="455"/>
+      <c r="L35" s="455"/>
+      <c r="M35" s="455"/>
+      <c r="N35" s="455"/>
+      <c r="O35" s="455"/>
+      <c r="P35" s="455"/>
+      <c r="Q35" s="455"/>
+      <c r="R35" s="440"/>
     </row>
     <row r="36" spans="1:20" ht="15.75" thickBot="1">
       <c r="A36" s="28" t="s">

</xml_diff>

<commit_message>
method declaration and return
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" tabRatio="601" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" tabRatio="601" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="pc-basics" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4792" uniqueCount="2513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4820" uniqueCount="2517">
   <si>
     <t>USER</t>
   </si>
@@ -7977,6 +7977,18 @@
   </si>
   <si>
     <t>when we run out of memory - clean up/delete/remove unused unreferenced data from memory</t>
+  </si>
+  <si>
+    <t>FBCust f2;</t>
+  </si>
+  <si>
+    <t>declared and initialized</t>
+  </si>
+  <si>
+    <t>declared</t>
+  </si>
+  <si>
+    <t>null = nothing / no reference / no memory address</t>
   </si>
 </sst>
 </file>
@@ -8695,7 +8707,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="491">
+  <cellXfs count="492">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -9535,6 +9547,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -9605,10 +9621,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -9656,7 +9672,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10013,13 +10028,13 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="15.75" thickBot="1">
-      <c r="H3" s="455" t="s">
+      <c r="H3" s="457" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="456"/>
-      <c r="J3" s="456"/>
-      <c r="K3" s="456"/>
-      <c r="L3" s="457"/>
+      <c r="I3" s="458"/>
+      <c r="J3" s="458"/>
+      <c r="K3" s="458"/>
+      <c r="L3" s="459"/>
       <c r="Q3" t="s">
         <v>2051</v>
       </c>
@@ -10048,20 +10063,20 @@
       <c r="F6" s="4" t="s">
         <v>1653</v>
       </c>
-      <c r="G6" s="458" t="s">
+      <c r="G6" s="460" t="s">
         <v>1173</v>
       </c>
-      <c r="H6" s="459"/>
+      <c r="H6" s="461"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="458" t="s">
+      <c r="J6" s="460" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="459"/>
+      <c r="K6" s="461"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="458" t="s">
+      <c r="M6" s="460" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="459"/>
+      <c r="N6" s="461"/>
       <c r="P6" t="s">
         <v>2043</v>
       </c>
@@ -10092,20 +10107,20 @@
       <c r="F8" s="4" t="s">
         <v>1200</v>
       </c>
-      <c r="G8" s="460" t="s">
+      <c r="G8" s="462" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="461"/>
+      <c r="H8" s="463"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="460" t="s">
+      <c r="J8" s="462" t="s">
         <v>5</v>
       </c>
-      <c r="K8" s="461"/>
+      <c r="K8" s="463"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="460" t="s">
+      <c r="M8" s="462" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="461"/>
+      <c r="N8" s="463"/>
       <c r="P8" t="s">
         <v>2045</v>
       </c>
@@ -10131,29 +10146,29 @@
       <c r="Q9" s="119"/>
     </row>
     <row r="10" spans="2:18">
-      <c r="F10" s="451" t="s">
+      <c r="F10" s="453" t="s">
         <v>1664</v>
       </c>
-      <c r="G10" s="452"/>
-      <c r="H10" s="452"/>
-      <c r="I10" s="452"/>
-      <c r="J10" s="452"/>
-      <c r="K10" s="452"/>
-      <c r="L10" s="452"/>
-      <c r="M10" s="452"/>
-      <c r="N10" s="452"/>
+      <c r="G10" s="454"/>
+      <c r="H10" s="454"/>
+      <c r="I10" s="454"/>
+      <c r="J10" s="454"/>
+      <c r="K10" s="454"/>
+      <c r="L10" s="454"/>
+      <c r="M10" s="454"/>
+      <c r="N10" s="454"/>
       <c r="Q10" s="119"/>
     </row>
     <row r="11" spans="2:18" ht="15.75" thickBot="1">
-      <c r="F11" s="453"/>
-      <c r="G11" s="454"/>
-      <c r="H11" s="454"/>
-      <c r="I11" s="454"/>
-      <c r="J11" s="454"/>
-      <c r="K11" s="454"/>
-      <c r="L11" s="454"/>
-      <c r="M11" s="454"/>
-      <c r="N11" s="454"/>
+      <c r="F11" s="455"/>
+      <c r="G11" s="456"/>
+      <c r="H11" s="456"/>
+      <c r="I11" s="456"/>
+      <c r="J11" s="456"/>
+      <c r="K11" s="456"/>
+      <c r="L11" s="456"/>
+      <c r="M11" s="456"/>
+      <c r="N11" s="456"/>
     </row>
     <row r="12" spans="2:18">
       <c r="D12" s="103" t="s">
@@ -10406,8 +10421,8 @@
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75" thickBot="1">
-      <c r="D23" s="449"/>
-      <c r="E23" s="450"/>
+      <c r="D23" s="451"/>
+      <c r="E23" s="452"/>
       <c r="F23" s="118"/>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
@@ -20651,34 +20666,34 @@
       <c r="E10" t="s">
         <v>1829</v>
       </c>
-      <c r="G10" s="462" t="s">
+      <c r="G10" s="464" t="s">
         <v>1836</v>
       </c>
-      <c r="H10" s="463"/>
-      <c r="I10" s="464"/>
+      <c r="H10" s="465"/>
+      <c r="I10" s="466"/>
       <c r="K10" s="28" t="s">
         <v>1846</v>
       </c>
       <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="G11" s="465"/>
-      <c r="H11" s="466"/>
-      <c r="I11" s="467"/>
+      <c r="G11" s="467"/>
+      <c r="H11" s="468"/>
+      <c r="I11" s="469"/>
       <c r="K11" s="31"/>
       <c r="L11" s="32"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1">
-      <c r="G12" s="465"/>
-      <c r="H12" s="466"/>
-      <c r="I12" s="467"/>
+      <c r="G12" s="467"/>
+      <c r="H12" s="468"/>
+      <c r="I12" s="469"/>
       <c r="K12" s="33"/>
       <c r="L12" s="35"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1">
-      <c r="G13" s="468"/>
-      <c r="H13" s="469"/>
-      <c r="I13" s="470"/>
+      <c r="G13" s="470"/>
+      <c r="H13" s="471"/>
+      <c r="I13" s="472"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1">
       <c r="E14" t="s">
@@ -21607,7 +21622,7 @@
       </c>
       <c r="J3" s="83"/>
       <c r="K3" s="275"/>
-      <c r="L3" s="476" t="s">
+      <c r="L3" s="478" t="s">
         <v>1479</v>
       </c>
       <c r="M3" s="170"/>
@@ -21629,7 +21644,7 @@
       <c r="K4" s="69">
         <v>123</v>
       </c>
-      <c r="L4" s="477"/>
+      <c r="L4" s="479"/>
       <c r="M4" s="170"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
@@ -21649,12 +21664,12 @@
       <c r="K5" s="276" t="s">
         <v>1478</v>
       </c>
-      <c r="L5" s="477"/>
+      <c r="L5" s="479"/>
       <c r="M5" s="170"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1">
       <c r="F6" s="186"/>
-      <c r="L6" s="477"/>
+      <c r="L6" s="479"/>
       <c r="M6" s="170"/>
     </row>
     <row r="7" spans="1:13">
@@ -21667,7 +21682,7 @@
       </c>
       <c r="J7" s="83"/>
       <c r="K7" s="275"/>
-      <c r="L7" s="477"/>
+      <c r="L7" s="479"/>
       <c r="M7" s="170"/>
     </row>
     <row r="8" spans="1:13">
@@ -21685,7 +21700,7 @@
       <c r="K8" s="69">
         <v>111</v>
       </c>
-      <c r="L8" s="477"/>
+      <c r="L8" s="479"/>
       <c r="M8" s="170"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1">
@@ -21699,7 +21714,7 @@
       <c r="K9" s="260" t="s">
         <v>164</v>
       </c>
-      <c r="L9" s="477"/>
+      <c r="L9" s="479"/>
       <c r="M9" s="170"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1">
@@ -21707,7 +21722,7 @@
         <v>1462</v>
       </c>
       <c r="F10" s="186"/>
-      <c r="L10" s="477"/>
+      <c r="L10" s="479"/>
       <c r="M10" s="170"/>
     </row>
     <row r="11" spans="1:13">
@@ -21720,7 +21735,7 @@
       </c>
       <c r="J11" s="83"/>
       <c r="K11" s="275"/>
-      <c r="L11" s="477"/>
+      <c r="L11" s="479"/>
       <c r="M11" s="170"/>
     </row>
     <row r="12" spans="1:13">
@@ -21734,7 +21749,7 @@
       <c r="K12" s="69">
         <v>222</v>
       </c>
-      <c r="L12" s="477"/>
+      <c r="L12" s="479"/>
       <c r="M12" s="170"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1">
@@ -21751,7 +21766,7 @@
       <c r="K13" s="260" t="s">
         <v>199</v>
       </c>
-      <c r="L13" s="478"/>
+      <c r="L13" s="480"/>
       <c r="M13" s="170"/>
     </row>
     <row r="14" spans="1:13">
@@ -21773,10 +21788,10 @@
       <c r="D15" s="255"/>
       <c r="E15" s="255"/>
       <c r="F15" s="186"/>
-      <c r="J15" s="471" t="s">
+      <c r="J15" s="473" t="s">
         <v>1468</v>
       </c>
-      <c r="K15" s="471"/>
+      <c r="K15" s="473"/>
       <c r="L15" s="69" t="s">
         <v>536</v>
       </c>
@@ -21796,8 +21811,8 @@
       <c r="G16" s="96" t="s">
         <v>1470</v>
       </c>
-      <c r="J16" s="471"/>
-      <c r="K16" s="471"/>
+      <c r="J16" s="473"/>
+      <c r="K16" s="473"/>
       <c r="L16" s="69" t="s">
         <v>50</v>
       </c>
@@ -21875,48 +21890,48 @@
     <row r="22" spans="1:13">
       <c r="A22" s="96"/>
       <c r="B22" s="96"/>
-      <c r="K22" s="472"/>
+      <c r="K22" s="475"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="96"/>
       <c r="B23" s="96"/>
-      <c r="K23" s="473"/>
+      <c r="K23" s="474"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="96"/>
       <c r="B24" s="96"/>
-      <c r="K24" s="473"/>
+      <c r="K24" s="474"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="96"/>
       <c r="B25" s="96"/>
-      <c r="K25" s="473"/>
+      <c r="K25" s="474"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="96"/>
       <c r="B26" s="96"/>
-      <c r="K26" s="473"/>
+      <c r="K26" s="474"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="K27" s="473"/>
+      <c r="K27" s="474"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="K28" s="473"/>
+      <c r="K28" s="474"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="96"/>
-      <c r="K29" s="473"/>
+      <c r="K29" s="474"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="96"/>
-      <c r="K30" s="473"/>
+      <c r="K30" s="474"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="96"/>
-      <c r="K31" s="473"/>
+      <c r="K31" s="474"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="K32" s="473"/>
+      <c r="K32" s="474"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="272"/>
@@ -31487,18 +31502,18 @@
       </c>
     </row>
     <row r="8" spans="1:38">
-      <c r="B8" s="480" t="s">
+      <c r="B8" s="482" t="s">
         <v>1608</v>
       </c>
-      <c r="C8" s="480"/>
-      <c r="F8" s="480" t="s">
+      <c r="C8" s="482"/>
+      <c r="F8" s="482" t="s">
         <v>1609</v>
       </c>
-      <c r="G8" s="480"/>
-      <c r="I8" s="480" t="s">
+      <c r="G8" s="482"/>
+      <c r="I8" s="482" t="s">
         <v>1609</v>
       </c>
-      <c r="J8" s="480"/>
+      <c r="J8" s="482"/>
       <c r="M8" s="108"/>
       <c r="N8" s="39"/>
       <c r="AA8">
@@ -31518,18 +31533,18 @@
       </c>
     </row>
     <row r="9" spans="1:38">
-      <c r="F9" s="481" t="s">
+      <c r="F9" s="483" t="s">
         <v>1610</v>
       </c>
-      <c r="G9" s="481"/>
-      <c r="I9" s="481" t="s">
+      <c r="G9" s="483"/>
+      <c r="I9" s="483" t="s">
         <v>1249</v>
       </c>
-      <c r="J9" s="481"/>
-      <c r="M9" s="482" t="s">
+      <c r="J9" s="483"/>
+      <c r="M9" s="484" t="s">
         <v>1609</v>
       </c>
-      <c r="N9" s="482"/>
+      <c r="N9" s="484"/>
       <c r="P9" t="s">
         <v>2425</v>
       </c>
@@ -31580,19 +31595,19 @@
       </c>
     </row>
     <row r="11" spans="1:38">
-      <c r="E11" s="479" t="s">
+      <c r="E11" s="481" t="s">
         <v>1612</v>
       </c>
-      <c r="F11" s="479"/>
-      <c r="G11" s="479"/>
-      <c r="H11" s="479"/>
-      <c r="I11" s="479"/>
-      <c r="J11" s="479"/>
-      <c r="K11" s="479"/>
-      <c r="L11" s="479"/>
-      <c r="M11" s="479"/>
-      <c r="N11" s="479"/>
-      <c r="O11" s="479"/>
+      <c r="F11" s="481"/>
+      <c r="G11" s="481"/>
+      <c r="H11" s="481"/>
+      <c r="I11" s="481"/>
+      <c r="J11" s="481"/>
+      <c r="K11" s="481"/>
+      <c r="L11" s="481"/>
+      <c r="M11" s="481"/>
+      <c r="N11" s="481"/>
+      <c r="O11" s="481"/>
       <c r="AF11" s="104" t="s">
         <v>810</v>
       </c>
@@ -35128,10 +35143,10 @@
       </c>
     </row>
     <row r="241" spans="1:12">
-      <c r="C241" s="449" t="s">
+      <c r="C241" s="451" t="s">
         <v>1636</v>
       </c>
-      <c r="D241" s="449"/>
+      <c r="D241" s="451"/>
       <c r="E241" s="122" t="s">
         <v>30</v>
       </c>
@@ -35658,8 +35673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78:D81"/>
+    <sheetView topLeftCell="A97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -35693,7 +35708,7 @@
       <c r="E2" s="367" t="s">
         <v>781</v>
       </c>
-      <c r="F2" s="490" t="s">
+      <c r="F2" s="450" t="s">
         <v>2466</v>
       </c>
       <c r="G2" s="76"/>
@@ -35952,7 +35967,7 @@
       <c r="E19" s="367" t="s">
         <v>781</v>
       </c>
-      <c r="F19" s="490" t="s">
+      <c r="F19" s="450" t="s">
         <v>2466</v>
       </c>
       <c r="G19" s="76"/>
@@ -36255,7 +36270,7 @@
       <c r="E39" s="367" t="s">
         <v>781</v>
       </c>
-      <c r="F39" s="490" t="s">
+      <c r="F39" s="450" t="s">
         <v>2466</v>
       </c>
       <c r="G39" s="76"/>
@@ -36575,7 +36590,7 @@
       <c r="E59" s="367" t="s">
         <v>781</v>
       </c>
-      <c r="F59" s="490" t="s">
+      <c r="F59" s="450" t="s">
         <v>2466</v>
       </c>
       <c r="G59" s="76"/>
@@ -36883,7 +36898,7 @@
       <c r="F78" s="367" t="s">
         <v>781</v>
       </c>
-      <c r="G78" s="490" t="s">
+      <c r="G78" s="450" t="s">
         <v>2466</v>
       </c>
       <c r="H78" s="76"/>
@@ -37187,180 +37202,282 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:14">
       <c r="D97" s="440"/>
       <c r="E97" s="440"/>
       <c r="F97" s="96"/>
       <c r="I97" s="440"/>
       <c r="J97" s="440"/>
     </row>
-    <row r="98" spans="1:12">
-      <c r="D98" s="440"/>
-      <c r="E98" s="440"/>
-      <c r="F98" s="96"/>
-      <c r="G98" s="96"/>
-      <c r="H98" s="440"/>
-      <c r="I98" s="440"/>
-      <c r="J98" s="440"/>
-      <c r="K98" s="440"/>
-      <c r="L98" s="440"/>
-    </row>
-    <row r="99" spans="1:12">
-      <c r="A99" s="254"/>
-      <c r="D99" s="440"/>
-      <c r="E99" s="440"/>
-      <c r="F99" s="96"/>
-      <c r="G99" s="96"/>
-      <c r="H99" s="440"/>
-      <c r="I99" s="440"/>
-      <c r="J99" s="440"/>
-      <c r="K99" s="440"/>
-      <c r="L99" s="440"/>
-    </row>
-    <row r="100" spans="1:12">
-      <c r="D100" s="440"/>
-      <c r="E100" s="440"/>
-      <c r="F100" s="96"/>
-      <c r="G100" s="440"/>
-      <c r="H100" s="96"/>
-      <c r="I100" s="440"/>
-      <c r="J100" s="440"/>
-      <c r="K100" s="440"/>
-      <c r="L100" s="440"/>
-    </row>
-    <row r="101" spans="1:12">
-      <c r="C101" s="254"/>
-      <c r="D101" s="440"/>
-      <c r="F101" s="440"/>
-      <c r="G101" s="440"/>
-      <c r="H101" s="440"/>
-      <c r="I101" s="440"/>
-      <c r="J101" s="440"/>
-    </row>
-    <row r="102" spans="1:12">
-      <c r="E102" s="96"/>
-      <c r="G102" s="440"/>
-      <c r="H102" s="440"/>
-      <c r="I102" s="440"/>
-      <c r="J102" s="440"/>
-      <c r="K102" s="440"/>
-      <c r="L102" s="440"/>
-    </row>
-    <row r="103" spans="1:12">
-      <c r="C103" s="254"/>
-      <c r="E103" s="96"/>
-      <c r="F103" s="96"/>
-      <c r="G103" s="440"/>
-      <c r="H103" s="440"/>
-      <c r="I103" s="440"/>
-      <c r="J103" s="440"/>
-      <c r="K103" s="440"/>
-      <c r="L103" s="440"/>
-    </row>
-    <row r="104" spans="1:12">
-      <c r="F104" s="440"/>
-      <c r="G104" s="96"/>
-      <c r="H104" s="440"/>
-      <c r="I104" s="440"/>
-      <c r="J104" s="440"/>
-      <c r="K104" s="440"/>
-      <c r="L104" s="440"/>
-    </row>
-    <row r="105" spans="1:12">
-      <c r="E105" s="96"/>
-      <c r="F105" s="440"/>
-      <c r="G105" s="106"/>
-      <c r="H105" s="440"/>
-      <c r="I105" s="96"/>
-      <c r="J105" s="440"/>
-      <c r="K105" s="440"/>
-      <c r="L105" s="440"/>
-    </row>
-    <row r="106" spans="1:12">
-      <c r="D106" s="96"/>
-      <c r="E106" s="96"/>
-      <c r="F106" s="440"/>
-      <c r="G106" s="440"/>
-      <c r="H106" s="440"/>
-      <c r="I106" s="96"/>
-      <c r="J106" s="440"/>
-      <c r="K106" s="440"/>
-      <c r="L106" s="440"/>
-    </row>
-    <row r="107" spans="1:12">
-      <c r="D107" s="96"/>
-      <c r="F107" s="96"/>
-      <c r="G107" s="440"/>
+    <row r="98" spans="1:14" ht="15.75" thickBot="1">
+      <c r="B98" s="254" t="s">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" ht="15.75" thickBot="1">
+      <c r="B99" s="36" t="s">
+        <v>2478</v>
+      </c>
+      <c r="C99" s="313"/>
+      <c r="F99" s="367" t="s">
+        <v>781</v>
+      </c>
+      <c r="G99" s="450" t="s">
+        <v>2466</v>
+      </c>
+      <c r="H99" s="76"/>
+      <c r="I99" s="76"/>
+      <c r="J99" s="76"/>
+      <c r="K99" s="76"/>
+      <c r="L99" s="76"/>
+      <c r="M99" s="76"/>
+      <c r="N99" s="77"/>
+    </row>
+    <row r="100" spans="1:14">
+      <c r="B100" s="313"/>
+      <c r="C100" s="313" t="s">
+        <v>84</v>
+      </c>
+      <c r="E100" s="449"/>
+      <c r="F100" s="186" t="s">
+        <v>2484</v>
+      </c>
+      <c r="G100" s="96" t="s">
+        <v>832</v>
+      </c>
+      <c r="J100" s="449"/>
+      <c r="K100" s="449" t="s">
+        <v>832</v>
+      </c>
+      <c r="L100" s="83"/>
+      <c r="M100" s="84"/>
+      <c r="N100" s="70"/>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="A101" s="254"/>
+      <c r="C101" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="E101" s="449"/>
+      <c r="F101" s="186" t="s">
+        <v>2485</v>
+      </c>
+      <c r="G101" s="96" t="s">
+        <v>134</v>
+      </c>
+      <c r="H101" s="96"/>
+      <c r="I101" s="449"/>
+      <c r="J101" s="449"/>
+      <c r="K101" s="449"/>
+      <c r="L101" s="186" t="s">
+        <v>32</v>
+      </c>
+      <c r="M101" s="170" t="s">
+        <v>132</v>
+      </c>
+      <c r="N101" s="170"/>
+    </row>
+    <row r="102" spans="1:14" ht="15.75" thickBot="1">
+      <c r="B102" s="313" t="s">
+        <v>278</v>
+      </c>
+      <c r="C102" s="313"/>
+      <c r="E102" s="449"/>
+      <c r="F102" s="316"/>
+      <c r="G102" s="96"/>
+      <c r="H102" s="96"/>
+      <c r="I102" s="449"/>
+      <c r="J102" s="449"/>
+      <c r="K102" s="449"/>
+      <c r="L102" s="187" t="s">
+        <v>41</v>
+      </c>
+      <c r="M102" s="188">
+        <v>10</v>
+      </c>
+      <c r="N102" s="170"/>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="B103" s="313" t="s">
+        <v>2514</v>
+      </c>
+      <c r="C103" s="313"/>
+      <c r="E103" s="449"/>
+      <c r="F103" s="186"/>
+      <c r="G103" s="96" t="s">
+        <v>2516</v>
+      </c>
+      <c r="H103" s="449"/>
+      <c r="I103" s="96"/>
+      <c r="J103" s="449"/>
+      <c r="K103" s="449"/>
+      <c r="L103" s="449"/>
+      <c r="M103" s="449"/>
+      <c r="N103" s="170"/>
+    </row>
+    <row r="104" spans="1:14">
+      <c r="B104" s="36" t="s">
+        <v>2480</v>
+      </c>
+      <c r="C104" s="313"/>
+      <c r="E104" s="449"/>
+      <c r="F104" s="78"/>
+      <c r="G104" s="255"/>
+      <c r="H104" s="255"/>
+      <c r="I104" s="255"/>
+      <c r="J104" s="449"/>
+      <c r="K104" s="255"/>
+      <c r="L104" s="255"/>
+      <c r="M104" s="255"/>
+      <c r="N104" s="170"/>
+    </row>
+    <row r="105" spans="1:14">
+      <c r="F105" s="310"/>
+      <c r="G105" s="255"/>
+      <c r="H105" s="255"/>
+      <c r="I105" s="255"/>
+      <c r="J105" s="449"/>
+      <c r="K105" s="255"/>
+      <c r="L105" s="255"/>
+      <c r="M105" s="255"/>
+      <c r="N105" s="170"/>
+    </row>
+    <row r="106" spans="1:14">
+      <c r="B106" s="36" t="s">
+        <v>2515</v>
+      </c>
+      <c r="F106" s="310"/>
+      <c r="G106" s="255"/>
+      <c r="H106" s="255"/>
+      <c r="I106" s="255"/>
+      <c r="J106" s="449"/>
+      <c r="K106" s="255"/>
+      <c r="L106" s="255"/>
+      <c r="M106" s="255"/>
+      <c r="N106" s="170"/>
+    </row>
+    <row r="107" spans="1:14">
+      <c r="B107" s="36" t="s">
+        <v>2513</v>
+      </c>
+      <c r="F107" s="78"/>
+      <c r="G107" s="96"/>
       <c r="H107" s="96"/>
-      <c r="I107" s="440"/>
-      <c r="J107" s="96"/>
-      <c r="K107" s="440"/>
-      <c r="L107" s="440"/>
-    </row>
-    <row r="108" spans="1:12">
-      <c r="E108" s="440"/>
-      <c r="F108" s="96"/>
-      <c r="G108" s="440"/>
-      <c r="H108" s="440"/>
-      <c r="I108" s="440"/>
-      <c r="J108" s="440"/>
-      <c r="K108" s="440"/>
-      <c r="L108" s="440"/>
-    </row>
-    <row r="109" spans="1:12">
+      <c r="I107" s="449"/>
+      <c r="J107" s="449"/>
+      <c r="K107" s="255"/>
+      <c r="L107" s="277"/>
+      <c r="M107" s="255"/>
+      <c r="N107" s="170"/>
+    </row>
+    <row r="108" spans="1:14">
+      <c r="F108" s="310"/>
+      <c r="G108" s="449"/>
+      <c r="H108" s="106"/>
+      <c r="I108" s="449"/>
+      <c r="J108" s="96"/>
+      <c r="K108" s="255"/>
+      <c r="L108" s="255"/>
+      <c r="M108" s="255"/>
+      <c r="N108" s="170"/>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="C109" s="182"/>
       <c r="E109" s="96"/>
-      <c r="F109" s="96"/>
-      <c r="G109" s="96"/>
-      <c r="H109" s="440"/>
-      <c r="I109" s="440"/>
-      <c r="J109" s="440"/>
-      <c r="K109" s="440"/>
-      <c r="L109" s="440"/>
-    </row>
-    <row r="110" spans="1:12">
-      <c r="E110" s="440"/>
-      <c r="F110" s="440"/>
-      <c r="G110" s="440"/>
-      <c r="H110" s="440"/>
-      <c r="I110" s="440"/>
-      <c r="J110" s="440"/>
-      <c r="K110" s="440"/>
-      <c r="L110" s="440"/>
-    </row>
-    <row r="112" spans="1:12">
-      <c r="C112" s="374"/>
-    </row>
-    <row r="116" spans="1:12">
-      <c r="D116" s="440"/>
-      <c r="E116" s="440"/>
-      <c r="F116" s="96"/>
-      <c r="I116" s="440"/>
-      <c r="J116" s="440"/>
-    </row>
-    <row r="117" spans="1:12">
-      <c r="D117" s="440"/>
-      <c r="E117" s="440"/>
-      <c r="F117" s="96"/>
-      <c r="G117" s="96"/>
-      <c r="H117" s="440"/>
-      <c r="I117" s="440"/>
-      <c r="J117" s="440"/>
-      <c r="K117" s="440"/>
-      <c r="L117" s="440"/>
-    </row>
-    <row r="118" spans="1:12">
-      <c r="A118" s="254"/>
-      <c r="D118" s="440"/>
-      <c r="E118" s="440"/>
+      <c r="F109" s="310" t="s">
+        <v>136</v>
+      </c>
+      <c r="G109" s="449"/>
+      <c r="H109" s="449" t="s">
+        <v>2486</v>
+      </c>
+      <c r="I109" s="449"/>
+      <c r="J109" s="96"/>
+      <c r="K109" s="255"/>
+      <c r="L109" s="255"/>
+      <c r="M109" s="255"/>
+      <c r="N109" s="170"/>
+    </row>
+    <row r="110" spans="1:14">
+      <c r="C110" s="182"/>
+      <c r="E110" s="449"/>
+      <c r="F110" s="310" t="s">
+        <v>2488</v>
+      </c>
+      <c r="G110" s="96"/>
+      <c r="H110" s="449" t="s">
+        <v>2490</v>
+      </c>
+      <c r="I110" s="449"/>
+      <c r="J110" s="449" t="s">
+        <v>34</v>
+      </c>
+      <c r="K110" s="255"/>
+      <c r="L110" s="255"/>
+      <c r="M110" s="255"/>
+      <c r="N110" s="170"/>
+    </row>
+    <row r="111" spans="1:14">
+      <c r="C111" s="182"/>
+      <c r="E111" s="449"/>
+      <c r="F111" s="186"/>
+      <c r="G111" s="96"/>
+      <c r="H111" s="449" t="s">
+        <v>2487</v>
+      </c>
+      <c r="I111" s="449"/>
+      <c r="J111" s="449"/>
+      <c r="K111" s="449"/>
+      <c r="L111" s="449"/>
+      <c r="M111" s="449"/>
+      <c r="N111" s="170"/>
+    </row>
+    <row r="112" spans="1:14">
+      <c r="C112" s="182"/>
+      <c r="E112" s="449"/>
+      <c r="F112" s="310"/>
+      <c r="G112" s="449"/>
+      <c r="H112" s="96"/>
+      <c r="I112" s="449"/>
+      <c r="J112" s="449" t="s">
+        <v>2511</v>
+      </c>
+      <c r="K112" s="449"/>
+      <c r="L112" s="449"/>
+      <c r="M112" s="449"/>
+      <c r="N112" s="170"/>
+    </row>
+    <row r="113" spans="1:14" ht="15.75" thickBot="1">
+      <c r="E113" s="449"/>
+      <c r="F113" s="428" t="s">
+        <v>2512</v>
+      </c>
+      <c r="G113" s="260"/>
+      <c r="H113" s="260"/>
+      <c r="I113" s="260"/>
+      <c r="J113" s="260"/>
+      <c r="K113" s="260"/>
+      <c r="L113" s="260"/>
+      <c r="M113" s="260"/>
+      <c r="N113" s="188"/>
+    </row>
+    <row r="114" spans="1:14">
+      <c r="E114" s="449"/>
+    </row>
+    <row r="116" spans="1:14">
+      <c r="A116" s="254"/>
+      <c r="C116" s="138"/>
+      <c r="D116" s="138"/>
+      <c r="N116" s="449"/>
+    </row>
+    <row r="118" spans="1:14">
+      <c r="D118" s="449"/>
+      <c r="E118" s="449"/>
       <c r="F118" s="96"/>
-      <c r="G118" s="96"/>
-      <c r="H118" s="440"/>
-      <c r="I118" s="440"/>
-      <c r="J118" s="440"/>
-      <c r="K118" s="440"/>
-      <c r="L118" s="440"/>
-    </row>
-    <row r="119" spans="1:12">
+      <c r="I118" s="449"/>
+      <c r="J118" s="449"/>
+    </row>
+    <row r="119" spans="1:14">
       <c r="D119" s="440"/>
       <c r="E119" s="440"/>
       <c r="F119" s="96"/>
@@ -37371,7 +37488,7 @@
       <c r="K119" s="440"/>
       <c r="L119" s="440"/>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:14">
       <c r="C120" s="254"/>
       <c r="D120" s="440"/>
       <c r="F120" s="440"/>
@@ -37380,7 +37497,7 @@
       <c r="I120" s="440"/>
       <c r="J120" s="440"/>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:14">
       <c r="E121" s="440"/>
       <c r="F121" s="440"/>
       <c r="G121" s="440"/>
@@ -37390,7 +37507,7 @@
       <c r="K121" s="440"/>
       <c r="L121" s="440"/>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:14">
       <c r="C122" s="254"/>
       <c r="D122" s="440"/>
       <c r="E122" s="440"/>
@@ -37401,7 +37518,7 @@
       <c r="K122" s="440"/>
       <c r="L122" s="440"/>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:14">
       <c r="F123" s="440"/>
       <c r="G123" s="96"/>
       <c r="H123" s="440"/>
@@ -37410,7 +37527,7 @@
       <c r="K123" s="440"/>
       <c r="L123" s="440"/>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:14">
       <c r="E124" s="440"/>
       <c r="F124" s="440"/>
       <c r="G124" s="106"/>
@@ -37420,7 +37537,7 @@
       <c r="K124" s="440"/>
       <c r="L124" s="440"/>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:14">
       <c r="D125" s="440"/>
       <c r="E125" s="440"/>
       <c r="F125" s="440"/>
@@ -37430,7 +37547,7 @@
       <c r="K125" s="440"/>
       <c r="L125" s="440"/>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:14">
       <c r="D126" s="96"/>
       <c r="F126" s="96"/>
       <c r="G126" s="440"/>
@@ -37440,7 +37557,7 @@
       <c r="K126" s="440"/>
       <c r="L126" s="440"/>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" spans="1:14">
       <c r="E127" s="440"/>
       <c r="F127" s="440"/>
       <c r="G127" s="440"/>
@@ -37450,7 +37567,7 @@
       <c r="K127" s="440"/>
       <c r="L127" s="440"/>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" spans="1:14">
       <c r="D128" s="440"/>
       <c r="E128" s="440"/>
       <c r="F128" s="440"/>
@@ -38013,10 +38130,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:21">
-      <c r="C2" s="483" t="s">
+      <c r="C2" s="485" t="s">
         <v>1312</v>
       </c>
-      <c r="D2" s="483"/>
+      <c r="D2" s="485"/>
       <c r="F2" s="25" t="s">
         <v>2028</v>
       </c>
@@ -39112,10 +39229,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="2:13">
-      <c r="B1" s="484" t="s">
+      <c r="B1" s="486" t="s">
         <v>1312</v>
       </c>
-      <c r="C1" s="484"/>
+      <c r="C1" s="486"/>
       <c r="E1" t="s">
         <v>1313</v>
       </c>
@@ -40537,18 +40654,18 @@
   <sheetData>
     <row r="2" spans="2:17" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:17" ht="15.75" thickBot="1">
-      <c r="B3" s="485" t="s">
+      <c r="B3" s="487" t="s">
         <v>1337</v>
       </c>
-      <c r="C3" s="486"/>
-      <c r="D3" s="486"/>
-      <c r="E3" s="486"/>
-      <c r="F3" s="486"/>
-      <c r="G3" s="486"/>
-      <c r="H3" s="486"/>
-      <c r="I3" s="486"/>
-      <c r="J3" s="486"/>
-      <c r="K3" s="487"/>
+      <c r="C3" s="488"/>
+      <c r="D3" s="488"/>
+      <c r="E3" s="488"/>
+      <c r="F3" s="488"/>
+      <c r="G3" s="488"/>
+      <c r="H3" s="488"/>
+      <c r="I3" s="488"/>
+      <c r="J3" s="488"/>
+      <c r="K3" s="489"/>
     </row>
     <row r="4" spans="2:17" ht="15.75" thickBot="1">
       <c r="G4" t="s">
@@ -40663,24 +40780,24 @@
       <c r="L12" s="25"/>
     </row>
     <row r="15" spans="2:17">
-      <c r="B15" s="488" t="s">
+      <c r="B15" s="490" t="s">
         <v>1338</v>
       </c>
-      <c r="C15" s="489"/>
-      <c r="D15" s="489"/>
-      <c r="E15" s="489"/>
-      <c r="F15" s="489"/>
-      <c r="G15" s="489"/>
-      <c r="H15" s="489"/>
-      <c r="I15" s="489"/>
-      <c r="J15" s="489"/>
-      <c r="K15" s="489"/>
-      <c r="L15" s="489"/>
-      <c r="M15" s="489"/>
-      <c r="N15" s="489"/>
-      <c r="O15" s="489"/>
-      <c r="P15" s="489"/>
-      <c r="Q15" s="489"/>
+      <c r="C15" s="491"/>
+      <c r="D15" s="491"/>
+      <c r="E15" s="491"/>
+      <c r="F15" s="491"/>
+      <c r="G15" s="491"/>
+      <c r="H15" s="491"/>
+      <c r="I15" s="491"/>
+      <c r="J15" s="491"/>
+      <c r="K15" s="491"/>
+      <c r="L15" s="491"/>
+      <c r="M15" s="491"/>
+      <c r="N15" s="491"/>
+      <c r="O15" s="491"/>
+      <c r="P15" s="491"/>
+      <c r="Q15" s="491"/>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1"/>
     <row r="17" spans="1:17">
@@ -41740,80 +41857,75 @@
       <c r="M214" s="362"/>
     </row>
     <row r="223" spans="4:13">
-      <c r="D223" s="471"/>
-      <c r="E223" s="471"/>
+      <c r="D223" s="473"/>
+      <c r="E223" s="473"/>
     </row>
     <row r="227" spans="4:11">
-      <c r="D227" s="471"/>
-      <c r="E227" s="471"/>
-      <c r="G227" s="471"/>
-      <c r="H227" s="471"/>
-      <c r="J227" s="471"/>
-      <c r="K227" s="471"/>
+      <c r="D227" s="473"/>
+      <c r="E227" s="473"/>
+      <c r="G227" s="473"/>
+      <c r="H227" s="473"/>
+      <c r="J227" s="473"/>
+      <c r="K227" s="473"/>
     </row>
     <row r="273" spans="2:9">
-      <c r="D273" s="473"/>
+      <c r="D273" s="474"/>
     </row>
     <row r="274" spans="2:9">
-      <c r="D274" s="473"/>
+      <c r="D274" s="474"/>
     </row>
     <row r="275" spans="2:9">
-      <c r="D275" s="473"/>
+      <c r="D275" s="474"/>
     </row>
     <row r="276" spans="2:9">
-      <c r="D276" s="473"/>
+      <c r="D276" s="474"/>
     </row>
     <row r="277" spans="2:9">
-      <c r="D277" s="473"/>
+      <c r="D277" s="474"/>
     </row>
     <row r="278" spans="2:9">
-      <c r="D278" s="473"/>
+      <c r="D278" s="474"/>
     </row>
     <row r="287" spans="2:9">
-      <c r="B287" s="472"/>
-      <c r="C287" s="471"/>
-      <c r="D287" s="471"/>
+      <c r="B287" s="475"/>
+      <c r="C287" s="473"/>
+      <c r="D287" s="473"/>
     </row>
     <row r="288" spans="2:9">
-      <c r="B288" s="473"/>
-      <c r="I288" s="472"/>
+      <c r="B288" s="474"/>
+      <c r="I288" s="475"/>
     </row>
     <row r="289" spans="2:14">
-      <c r="B289" s="473"/>
-      <c r="I289" s="473"/>
-      <c r="N289" s="472"/>
+      <c r="B289" s="474"/>
+      <c r="I289" s="474"/>
+      <c r="N289" s="475"/>
     </row>
     <row r="290" spans="2:14">
-      <c r="B290" s="473"/>
-      <c r="F290" s="471"/>
-      <c r="G290" s="471"/>
-      <c r="H290" s="471"/>
-      <c r="I290" s="473"/>
-      <c r="N290" s="473"/>
+      <c r="B290" s="474"/>
+      <c r="F290" s="473"/>
+      <c r="G290" s="473"/>
+      <c r="H290" s="473"/>
+      <c r="I290" s="474"/>
+      <c r="N290" s="474"/>
     </row>
     <row r="291" spans="2:14">
-      <c r="B291" s="473"/>
-      <c r="C291" s="471"/>
-      <c r="D291" s="471"/>
-      <c r="I291" s="473"/>
-      <c r="K291" s="471"/>
-      <c r="L291" s="471"/>
-      <c r="M291" s="471"/>
-      <c r="N291" s="473"/>
+      <c r="B291" s="474"/>
+      <c r="C291" s="473"/>
+      <c r="D291" s="473"/>
+      <c r="I291" s="474"/>
+      <c r="K291" s="473"/>
+      <c r="L291" s="473"/>
+      <c r="M291" s="473"/>
+      <c r="N291" s="474"/>
     </row>
     <row r="292" spans="2:14">
-      <c r="N292" s="473"/>
+      <c r="N292" s="474"/>
     </row>
     <row r="306" spans="6:6">
       <c r="F306" s="250"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G227:H227"/>
-    <mergeCell ref="J227:K227"/>
-    <mergeCell ref="D227:E227"/>
-    <mergeCell ref="D223:E223"/>
-    <mergeCell ref="D273:D278"/>
     <mergeCell ref="C287:D287"/>
     <mergeCell ref="C291:D291"/>
     <mergeCell ref="B287:B291"/>
@@ -41821,6 +41933,11 @@
     <mergeCell ref="N289:N292"/>
     <mergeCell ref="I288:I291"/>
     <mergeCell ref="F290:H290"/>
+    <mergeCell ref="G227:H227"/>
+    <mergeCell ref="J227:K227"/>
+    <mergeCell ref="D227:E227"/>
+    <mergeCell ref="D223:E223"/>
+    <mergeCell ref="D273:D278"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -43148,8 +43265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43488,8 +43605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q107"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="N71" sqref="M71:N71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44550,23 +44667,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="475" t="s">
+      <c r="A1" s="477" t="s">
         <v>1094</v>
       </c>
-      <c r="B1" s="475"/>
-      <c r="C1" s="475"/>
-      <c r="D1" s="475"/>
-      <c r="E1" s="475"/>
-      <c r="F1" s="475"/>
-      <c r="I1" s="475" t="s">
+      <c r="B1" s="477"/>
+      <c r="C1" s="477"/>
+      <c r="D1" s="477"/>
+      <c r="E1" s="477"/>
+      <c r="F1" s="477"/>
+      <c r="I1" s="477" t="s">
         <v>1104</v>
       </c>
-      <c r="J1" s="475"/>
-      <c r="K1" s="475"/>
-      <c r="L1" s="475"/>
-      <c r="M1" s="475"/>
-      <c r="N1" s="475"/>
-      <c r="O1" s="475"/>
+      <c r="J1" s="477"/>
+      <c r="K1" s="477"/>
+      <c r="L1" s="477"/>
+      <c r="M1" s="477"/>
+      <c r="N1" s="477"/>
+      <c r="O1" s="477"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -44716,28 +44833,28 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A12" s="458" t="s">
+      <c r="A12" s="460" t="s">
         <v>1106</v>
       </c>
-      <c r="B12" s="474"/>
-      <c r="C12" s="474"/>
-      <c r="D12" s="474"/>
-      <c r="E12" s="474"/>
-      <c r="F12" s="474"/>
-      <c r="G12" s="474"/>
-      <c r="H12" s="459"/>
-      <c r="I12" s="458" t="s">
+      <c r="B12" s="476"/>
+      <c r="C12" s="476"/>
+      <c r="D12" s="476"/>
+      <c r="E12" s="476"/>
+      <c r="F12" s="476"/>
+      <c r="G12" s="476"/>
+      <c r="H12" s="461"/>
+      <c r="I12" s="460" t="s">
         <v>1106</v>
       </c>
-      <c r="J12" s="474"/>
-      <c r="K12" s="474"/>
-      <c r="L12" s="474"/>
-      <c r="M12" s="474"/>
-      <c r="N12" s="474"/>
-      <c r="O12" s="474"/>
-      <c r="P12" s="474"/>
-      <c r="Q12" s="474"/>
-      <c r="R12" s="459"/>
+      <c r="J12" s="476"/>
+      <c r="K12" s="476"/>
+      <c r="L12" s="476"/>
+      <c r="M12" s="476"/>
+      <c r="N12" s="476"/>
+      <c r="O12" s="476"/>
+      <c r="P12" s="476"/>
+      <c r="Q12" s="476"/>
+      <c r="R12" s="461"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="28" t="s">
@@ -44965,14 +45082,14 @@
       <c r="R21" s="35"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="475" t="s">
+      <c r="A24" s="477" t="s">
         <v>1094</v>
       </c>
-      <c r="B24" s="475"/>
-      <c r="C24" s="475"/>
-      <c r="D24" s="475"/>
-      <c r="E24" s="475"/>
-      <c r="F24" s="475"/>
+      <c r="B24" s="477"/>
+      <c r="C24" s="477"/>
+      <c r="D24" s="477"/>
+      <c r="E24" s="477"/>
+      <c r="F24" s="477"/>
       <c r="H24" s="194" t="s">
         <v>1104</v>
       </c>
@@ -44982,11 +45099,11 @@
       <c r="L24" s="194"/>
       <c r="M24" s="194"/>
       <c r="N24" s="194"/>
-      <c r="P24" s="475" t="s">
+      <c r="P24" s="477" t="s">
         <v>1142</v>
       </c>
-      <c r="Q24" s="475"/>
-      <c r="R24" s="475"/>
+      <c r="Q24" s="477"/>
+      <c r="R24" s="477"/>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="86" t="s">
@@ -45226,28 +45343,28 @@
       </c>
     </row>
     <row r="35" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A35" s="458" t="s">
+      <c r="A35" s="460" t="s">
         <v>1143</v>
       </c>
-      <c r="B35" s="474"/>
-      <c r="C35" s="474"/>
-      <c r="D35" s="474"/>
-      <c r="E35" s="474"/>
-      <c r="F35" s="474"/>
-      <c r="G35" s="474"/>
-      <c r="H35" s="459"/>
-      <c r="I35" s="458" t="s">
+      <c r="B35" s="476"/>
+      <c r="C35" s="476"/>
+      <c r="D35" s="476"/>
+      <c r="E35" s="476"/>
+      <c r="F35" s="476"/>
+      <c r="G35" s="476"/>
+      <c r="H35" s="461"/>
+      <c r="I35" s="460" t="s">
         <v>540</v>
       </c>
-      <c r="J35" s="474"/>
-      <c r="K35" s="474"/>
-      <c r="L35" s="474"/>
-      <c r="M35" s="474"/>
-      <c r="N35" s="474"/>
-      <c r="O35" s="474"/>
-      <c r="P35" s="474"/>
-      <c r="Q35" s="474"/>
-      <c r="R35" s="459"/>
+      <c r="J35" s="476"/>
+      <c r="K35" s="476"/>
+      <c r="L35" s="476"/>
+      <c r="M35" s="476"/>
+      <c r="N35" s="476"/>
+      <c r="O35" s="476"/>
+      <c r="P35" s="476"/>
+      <c r="Q35" s="476"/>
+      <c r="R35" s="461"/>
     </row>
     <row r="36" spans="1:20" ht="15.75" thickBot="1">
       <c r="A36" s="28" t="s">

</xml_diff>